<commit_message>
Fill all missings with MMI
</commit_message>
<xml_diff>
--- a/Model building/Results 20.xlsx
+++ b/Model building/Results 20.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A49B08-A327-4242-A2E6-C8D75616CADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="1275" windowWidth="21600" windowHeight="11280" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="1275" windowWidth="21600" windowHeight="10575" tabRatio="640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="21" r:id="rId1"/>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2325" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="71">
   <si>
     <t>Null Model</t>
   </si>
@@ -266,11 +265,14 @@
   <si>
     <t>All countries</t>
   </si>
+  <si>
+    <t>ESCS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -763,14 +765,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F4851D-80C2-4990-AB58-C13F9E65D56B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -780,10 +782,10 @@
     <col min="3" max="3" width="9.140625" style="11"/>
     <col min="4" max="4" width="8" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.5703125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="11"/>
-    <col min="7" max="7" width="7.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.5703125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="11"/>
+    <col min="9" max="9" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="11" customWidth="1"/>
     <col min="11" max="11" width="3.5703125" style="11" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="11"/>
@@ -900,37 +902,37 @@
         <v>5</v>
       </c>
       <c r="F4" s="11">
-        <v>451.73500000000001</v>
+        <v>449.92399999999998</v>
       </c>
       <c r="G4" s="11">
-        <v>1.7729999999999999</v>
+        <v>1.728</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="11">
-        <v>445.11200000000002</v>
+        <v>444.23700000000002</v>
       </c>
       <c r="J4" s="11">
-        <v>2.6080000000000001</v>
+        <v>2.5960000000000001</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="L4" s="11">
-        <v>491.35500000000002</v>
+        <v>484.48099999999999</v>
       </c>
       <c r="M4" s="11">
-        <v>4.1710000000000003</v>
+        <v>4.8419999999999996</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O4" s="11">
-        <v>396.42500000000001</v>
+        <v>392.88</v>
       </c>
       <c r="P4" s="11">
-        <v>14.348000000000001</v>
+        <v>14.074</v>
       </c>
       <c r="Q4" s="11" t="s">
         <v>5</v>
@@ -962,7 +964,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="11">
-        <v>-8.1000000000000003E-2</v>
+        <v>-6.7000000000000004E-2</v>
       </c>
       <c r="G6" s="11">
         <v>8.0000000000000002E-3</v>
@@ -971,7 +973,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="11">
-        <v>-3.5999999999999997E-2</v>
+        <v>-0.03</v>
       </c>
       <c r="J6" s="11">
         <v>1.0999999999999999E-2</v>
@@ -980,19 +982,19 @@
         <v>8</v>
       </c>
       <c r="L6" s="11">
-        <v>-3.1E-2</v>
+        <v>-0.03</v>
       </c>
       <c r="M6" s="11">
-        <v>1.2E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O6" s="11">
-        <v>-7.0000000000000001E-3</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
       <c r="P6" s="11">
-        <v>1.7999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1003,7 +1005,7 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14">
-        <v>-0.14099999999999999</v>
+        <v>-0.125</v>
       </c>
       <c r="G7" s="14">
         <v>8.0000000000000002E-3</v>
@@ -1012,7 +1014,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="14">
-        <v>-9.9000000000000005E-2</v>
+        <v>-0.09</v>
       </c>
       <c r="J7" s="14">
         <v>1.0999999999999999E-2</v>
@@ -1021,19 +1023,19 @@
         <v>5</v>
       </c>
       <c r="L7" s="14">
-        <v>-9.5000000000000001E-2</v>
+        <v>-0.09</v>
       </c>
       <c r="M7" s="14">
-        <v>1.2E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="N7" s="14" t="s">
         <v>5</v>
       </c>
       <c r="O7" s="14">
-        <v>-7.8E-2</v>
+        <v>-7.3999999999999996E-2</v>
       </c>
       <c r="P7" s="14">
-        <v>1.6E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="Q7" s="14" t="s">
         <v>5</v>
@@ -1047,7 +1049,7 @@
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
       <c r="F8" s="25">
-        <v>5.8999999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G8" s="25">
         <v>3.0000000000000001E-3</v>
@@ -1056,7 +1058,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="25">
-        <v>6.4000000000000001E-2</v>
+        <v>0.06</v>
       </c>
       <c r="J8" s="25">
         <v>4.0000000000000001E-3</v>
@@ -1065,7 +1067,7 @@
         <v>5</v>
       </c>
       <c r="L8" s="25">
-        <v>6.4000000000000001E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="M8" s="25">
         <v>4.0000000000000001E-3</v>
@@ -1074,7 +1076,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="25">
-        <v>7.0999999999999994E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="P8" s="25">
         <v>5.0000000000000001E-3</v>
@@ -1100,7 +1102,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="25">
-        <v>5.8000000000000003E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="J9" s="25">
         <v>3.0000000000000001E-3</v>
@@ -1109,7 +1111,7 @@
         <v>5</v>
       </c>
       <c r="L9" s="25">
-        <v>5.6000000000000001E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="M9" s="25">
         <v>3.0000000000000001E-3</v>
@@ -1118,7 +1120,7 @@
         <v>5</v>
       </c>
       <c r="O9" s="25">
-        <v>5.8000000000000003E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="P9" s="25">
         <v>5.0000000000000001E-3</v>
@@ -1135,16 +1137,16 @@
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
       <c r="F10" s="25">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G10" s="25">
         <v>2E-3</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="I10" s="25">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J10" s="25">
         <v>2E-3</v>
@@ -1153,7 +1155,7 @@
         <v>8</v>
       </c>
       <c r="L10" s="25">
-        <v>8.0000000000000002E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M10" s="25">
         <v>2E-3</v>
@@ -1162,7 +1164,7 @@
         <v>5</v>
       </c>
       <c r="O10" s="25">
-        <v>1.4E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="P10" s="25">
         <v>2E-3</v>
@@ -1176,7 +1178,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="11">
-        <v>9.8000000000000004E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="G11" s="11">
         <v>8.0000000000000002E-3</v>
@@ -1185,28 +1187,28 @@
         <v>5</v>
       </c>
       <c r="I11" s="11">
-        <v>6.9000000000000006E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="J11" s="11">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>5</v>
       </c>
       <c r="L11" s="11">
-        <v>6.2E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="M11" s="11">
-        <v>1.0999999999999999E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="N11" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O11" s="11">
-        <v>8.4000000000000005E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="P11" s="11">
-        <v>8.9999999999999993E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="Q11" s="11" t="s">
         <v>5</v>
@@ -1220,37 +1222,37 @@
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14">
-        <v>7.9000000000000001E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="G12" s="14">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>5</v>
       </c>
       <c r="I12" s="14">
-        <v>5.8999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="J12" s="14">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="K12" s="14" t="s">
         <v>5</v>
       </c>
       <c r="L12" s="14">
-        <v>5.3999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="M12" s="14">
-        <v>1.0999999999999999E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="N12" s="14" t="s">
         <v>5</v>
       </c>
       <c r="O12" s="14">
-        <v>7.0999999999999994E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="P12" s="14">
-        <v>8.9999999999999993E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="Q12" s="14" t="s">
         <v>5</v>
@@ -1264,7 +1266,7 @@
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
       <c r="F13" s="25">
-        <v>1.7999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G13" s="25">
         <v>2E-3</v>
@@ -1282,7 +1284,7 @@
         <v>5</v>
       </c>
       <c r="L13" s="25">
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="M13" s="25">
         <v>2E-3</v>
@@ -1294,10 +1296,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="P13" s="25">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="Q13" s="25" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1308,7 +1310,7 @@
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
       <c r="F14" s="25">
-        <v>1.9E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G14" s="25">
         <v>2E-3</v>
@@ -1326,7 +1328,7 @@
         <v>5</v>
       </c>
       <c r="L14" s="25">
-        <v>8.9999999999999993E-3</v>
+        <v>0.01</v>
       </c>
       <c r="M14" s="25">
         <v>2E-3</v>
@@ -1373,7 +1375,7 @@
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="25">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="P15" s="25">
         <v>1E-3</v>
@@ -1385,31 +1387,31 @@
         <v>15</v>
       </c>
       <c r="F16" s="11">
-        <v>1.4E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="G16" s="11">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I16" s="11">
-        <v>1.4999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="J16" s="11">
         <v>0.01</v>
       </c>
       <c r="L16" s="11">
-        <v>8.9999999999999993E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="M16" s="11">
-        <v>1.0999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="O16" s="11">
-        <v>3.5999999999999997E-2</v>
+        <v>0.03</v>
       </c>
       <c r="P16" s="11">
-        <v>1.4E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="Q16" s="11" t="s">
         <v>9</v>
@@ -1423,37 +1425,33 @@
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14">
-        <v>-0.02</v>
+        <v>-1.4E-2</v>
       </c>
       <c r="G17" s="14">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="I17" s="14">
-        <v>-1.9E-2</v>
+        <v>-1.4E-2</v>
       </c>
       <c r="J17" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>16</v>
-      </c>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="K17" s="14"/>
       <c r="L17" s="14">
-        <v>-2.1999999999999999E-2</v>
+        <v>-1.4E-2</v>
       </c>
       <c r="M17" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="N17" s="14" t="s">
-        <v>9</v>
-      </c>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="N17" s="14"/>
       <c r="O17" s="14">
-        <v>-4.0000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="P17" s="14">
-        <v>1.4E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="Q17" s="14"/>
     </row>
@@ -1465,16 +1463,16 @@
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
       <c r="F18" s="25">
-        <v>3.4000000000000002E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G18" s="25">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="H18" s="25" t="s">
         <v>5</v>
       </c>
       <c r="I18" s="25">
-        <v>3.4000000000000002E-2</v>
+        <v>0.03</v>
       </c>
       <c r="J18" s="25">
         <v>3.0000000000000001E-3</v>
@@ -1483,7 +1481,7 @@
         <v>5</v>
       </c>
       <c r="L18" s="25">
-        <v>3.1E-2</v>
+        <v>0.03</v>
       </c>
       <c r="M18" s="25">
         <v>3.0000000000000001E-3</v>
@@ -1492,10 +1490,10 @@
         <v>5</v>
       </c>
       <c r="O18" s="25">
-        <v>0.04</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="P18" s="25">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="Q18" s="25" t="s">
         <v>5</v>
@@ -1509,7 +1507,7 @@
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
       <c r="F19" s="25">
-        <v>0.03</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="G19" s="25">
         <v>2E-3</v>
@@ -1518,25 +1516,25 @@
         <v>5</v>
       </c>
       <c r="I19" s="25">
-        <v>2.8000000000000001E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="J19" s="25">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="K19" s="25" t="s">
         <v>5</v>
       </c>
       <c r="L19" s="25">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M19" s="25">
+        <v>2E-3</v>
+      </c>
+      <c r="N19" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="O19" s="25">
         <v>2.4E-2</v>
-      </c>
-      <c r="M19" s="25">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="N19" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="O19" s="25">
-        <v>2.5999999999999999E-2</v>
       </c>
       <c r="P19" s="25">
         <v>3.0000000000000001E-3</v>
@@ -1553,16 +1551,16 @@
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="25">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G20" s="25">
         <v>1E-3</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="I20" s="25">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J20" s="25">
         <v>2E-3</v>
@@ -1571,16 +1569,16 @@
         <v>8</v>
       </c>
       <c r="L20" s="25">
-        <v>7.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M20" s="25">
         <v>2E-3</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O20" s="25">
-        <v>1.4E-2</v>
+        <v>0.01</v>
       </c>
       <c r="P20" s="25">
         <v>2E-3</v>
@@ -1594,13 +1592,13 @@
         <v>19</v>
       </c>
       <c r="F21" s="11">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G21" s="11">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="I21" s="15">
-        <v>-3.9E-2</v>
+        <v>-3.7999999999999999E-2</v>
       </c>
       <c r="J21" s="15">
         <v>1.2E-2</v>
@@ -1609,7 +1607,7 @@
         <v>8</v>
       </c>
       <c r="L21" s="15">
-        <v>-4.1000000000000002E-2</v>
+        <v>-3.7999999999999999E-2</v>
       </c>
       <c r="M21" s="15">
         <v>1.2E-2</v>
@@ -1618,10 +1616,10 @@
         <v>8</v>
       </c>
       <c r="O21" s="15">
-        <v>-3.9E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="P21" s="15">
-        <v>1.4E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="Q21" s="11" t="s">
         <v>8</v>
@@ -1635,22 +1633,22 @@
         <v>0.08</v>
       </c>
       <c r="G22" s="11">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I22" s="15">
-        <v>1.4E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="J22" s="15">
         <v>1.2E-2</v>
       </c>
       <c r="L22" s="15">
-        <v>1.7000000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="M22" s="15">
-        <v>1.2999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="O22" s="15">
         <v>-2.1000000000000001E-2</v>
@@ -1667,57 +1665,60 @@
         <v>18</v>
       </c>
       <c r="F23" s="11">
-        <v>-0.01</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
       <c r="G23" s="11">
         <v>8.0000000000000002E-3</v>
       </c>
+      <c r="H23" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I23" s="11">
-        <v>1.4999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="J23" s="11">
         <v>0.01</v>
       </c>
       <c r="L23" s="11">
-        <v>8.9999999999999993E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M23" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="O23" s="11">
+        <v>1.9E-2</v>
+      </c>
+      <c r="P23" s="11">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="O23" s="11">
-        <v>2.3E-2</v>
-      </c>
-      <c r="P23" s="11">
-        <v>1.2E-2</v>
-      </c>
       <c r="Q23" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="F24" s="11">
-        <v>0.46</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="G24" s="11">
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="11">
-        <v>0.26200000000000001</v>
+        <v>0.245</v>
       </c>
       <c r="J24" s="11">
-        <v>1.4999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="K24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="L24" s="11">
-        <v>0.25700000000000001</v>
+        <v>0.245</v>
       </c>
       <c r="M24" s="11">
         <v>1.6E-2</v>
@@ -1726,10 +1727,10 @@
         <v>5</v>
       </c>
       <c r="O24" s="11">
-        <v>0.20799999999999999</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="P24" s="11">
-        <v>1.9E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="Q24" s="11" t="s">
         <v>5</v>
@@ -1761,19 +1762,19 @@
         <v>22</v>
       </c>
       <c r="L26" s="11">
-        <v>-0.249</v>
+        <v>-0.27900000000000003</v>
       </c>
       <c r="M26" s="11">
-        <v>0.06</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="N26" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O26" s="11">
-        <v>-0.25900000000000001</v>
+        <v>-0.27900000000000003</v>
       </c>
       <c r="P26" s="11">
-        <v>7.0999999999999994E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="Q26" s="11" t="s">
         <v>5</v>
@@ -1784,19 +1785,19 @@
         <v>23</v>
       </c>
       <c r="L27" s="11">
-        <v>0.29799999999999999</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="M27" s="11">
-        <v>6.5000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="N27" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O27" s="11">
-        <v>0.441</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="P27" s="11">
-        <v>6.5000000000000002E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="Q27" s="11" t="s">
         <v>5</v>
@@ -1809,22 +1810,19 @@
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="L28" s="11">
-        <v>-0.32</v>
+        <v>-0.27500000000000002</v>
       </c>
       <c r="M28" s="11">
-        <v>5.5E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="N28" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O28" s="11">
-        <v>-0.16400000000000001</v>
+        <v>-0.10199999999999999</v>
       </c>
       <c r="P28" s="11">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="Q28" s="11" t="s">
-        <v>8</v>
+        <v>5.8000000000000003E-2</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1832,19 +1830,19 @@
         <v>25</v>
       </c>
       <c r="L29" s="11">
-        <v>-0.29899999999999999</v>
+        <v>-0.28399999999999997</v>
       </c>
       <c r="M29" s="11">
-        <v>3.9E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="N29" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O29" s="11">
-        <v>-0.184</v>
+        <v>-0.157</v>
       </c>
       <c r="P29" s="11">
-        <v>4.1000000000000002E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="Q29" s="11" t="s">
         <v>5</v>
@@ -1855,7 +1853,7 @@
         <v>26</v>
       </c>
       <c r="L30" s="11">
-        <v>-0.121</v>
+        <v>-0.111</v>
       </c>
       <c r="M30" s="11">
         <v>2.8000000000000001E-2</v>
@@ -1864,10 +1862,10 @@
         <v>5</v>
       </c>
       <c r="O30" s="11">
-        <v>7.0000000000000001E-3</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="P30" s="11">
-        <v>7.6999999999999999E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1896,10 +1894,10 @@
         <v>68</v>
       </c>
       <c r="O32" s="11">
-        <v>0.69899999999999995</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="P32" s="11">
-        <v>8.8999999999999996E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="Q32" s="11" t="s">
         <v>5</v>
@@ -1916,38 +1914,38 @@
         <v>27</v>
       </c>
       <c r="C35" s="27">
-        <v>6117.3670000000002</v>
+        <v>6117.3689999999997</v>
       </c>
       <c r="D35" s="27">
         <v>292.91199999999998</v>
       </c>
       <c r="E35" s="27"/>
       <c r="F35" s="27">
-        <v>7450.9179999999997</v>
+        <v>7789.9570000000003</v>
       </c>
       <c r="G35" s="27">
-        <v>110.105</v>
+        <v>111.176</v>
       </c>
       <c r="H35" s="27"/>
       <c r="I35" s="27">
-        <v>5656.8310000000001</v>
+        <v>5760.9390000000003</v>
       </c>
       <c r="J35" s="27">
-        <v>127.946</v>
+        <v>129.51900000000001</v>
       </c>
       <c r="K35" s="27"/>
       <c r="L35" s="27">
-        <v>5645.8720000000003</v>
+        <v>5760.9690000000001</v>
       </c>
       <c r="M35" s="27">
-        <v>142.47399999999999</v>
+        <v>129.51499999999999</v>
       </c>
       <c r="N35" s="27"/>
       <c r="O35" s="27">
-        <v>5546.0590000000002</v>
+        <v>5742.1440000000002</v>
       </c>
       <c r="P35" s="27">
-        <v>220.578</v>
+        <v>249.886</v>
       </c>
       <c r="Q35" s="27"/>
     </row>
@@ -1957,34 +1955,34 @@
         <v>28</v>
       </c>
       <c r="C36" s="27">
-        <v>2657.4479999999999</v>
+        <v>2657.4430000000002</v>
       </c>
       <c r="D36" s="27">
-        <v>329.29599999999999</v>
+        <v>329.29399999999998</v>
       </c>
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
       <c r="I36" s="27">
-        <v>3113.0729999999999</v>
+        <v>3251.7449999999999</v>
       </c>
       <c r="J36" s="27">
-        <v>192.25200000000001</v>
+        <v>195.25800000000001</v>
       </c>
       <c r="K36" s="27"/>
       <c r="L36" s="27">
-        <v>1310.682</v>
+        <v>1621.6949999999999</v>
       </c>
       <c r="M36" s="27">
-        <v>134.083</v>
+        <v>142.679</v>
       </c>
       <c r="N36" s="27"/>
       <c r="O36" s="27">
-        <v>973.04</v>
+        <v>1064.1089999999999</v>
       </c>
       <c r="P36" s="27">
-        <v>126.85299999999999</v>
+        <v>130.85400000000001</v>
       </c>
       <c r="Q36" s="27"/>
     </row>
@@ -2010,10 +2008,10 @@
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
       <c r="O37" s="19">
-        <v>698.21</v>
+        <v>715.69200000000001</v>
       </c>
       <c r="P37" s="19">
-        <v>212.499</v>
+        <v>211.94499999999999</v>
       </c>
       <c r="Q37" s="19"/>
     </row>
@@ -2068,38 +2066,38 @@
         <v>32</v>
       </c>
       <c r="C40" s="23">
-        <v>1408122.2949999999</v>
+        <v>1408122.2930000001</v>
       </c>
       <c r="D40" s="23">
-        <v>377.19900000000001</v>
+        <v>377.19799999999998</v>
       </c>
       <c r="E40" s="23"/>
       <c r="F40" s="23">
-        <v>3227747.2170000002</v>
+        <v>3516405.7230000002</v>
       </c>
       <c r="G40" s="23">
-        <v>868.471</v>
+        <v>1347.971</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23">
-        <v>3260162.4759999998</v>
+        <v>3539126.6170000001</v>
       </c>
       <c r="J40" s="23">
-        <v>1165.9337</v>
+        <v>1692.1510000000001</v>
       </c>
       <c r="K40" s="23"/>
       <c r="L40" s="23">
-        <v>2749224.1949999998</v>
+        <v>3497150.173</v>
       </c>
       <c r="M40" s="23">
-        <v>1145.789</v>
+        <v>1608.317</v>
       </c>
       <c r="N40" s="23"/>
       <c r="O40" s="23">
-        <v>3005059.3020000001</v>
+        <v>3886028.93</v>
       </c>
       <c r="P40" s="23">
-        <v>434.31</v>
+        <v>616.88</v>
       </c>
       <c r="Q40" s="23"/>
     </row>
@@ -2109,38 +2107,38 @@
         <v>33</v>
       </c>
       <c r="C41" s="23">
-        <v>1408161.098</v>
+        <v>1408161.0959999999</v>
       </c>
       <c r="D41" s="23">
-        <v>377.19900000000001</v>
+        <v>377.19799999999998</v>
       </c>
       <c r="E41" s="23"/>
       <c r="F41" s="23">
-        <v>3228090.858</v>
+        <v>3516750.6779999998</v>
       </c>
       <c r="G41" s="23">
-        <v>868.471</v>
+        <v>1347.971</v>
       </c>
       <c r="H41" s="23"/>
       <c r="I41" s="23">
-        <v>3260706.5729999999</v>
+        <v>3539672.7960000001</v>
       </c>
       <c r="J41" s="23">
-        <v>1165.9369999999999</v>
+        <v>1592.1510000000001</v>
       </c>
       <c r="K41" s="23"/>
       <c r="L41" s="23">
-        <v>2749702.875</v>
+        <v>3497638.86</v>
       </c>
       <c r="M41" s="23">
-        <v>1145.789</v>
+        <v>1608.317</v>
       </c>
       <c r="N41" s="23"/>
       <c r="O41" s="23">
-        <v>3005591.52</v>
+        <v>3886572.1770000001</v>
       </c>
       <c r="P41" s="23">
-        <v>434.31</v>
+        <v>616.88</v>
       </c>
       <c r="Q41" s="23"/>
     </row>
@@ -2148,29 +2146,35 @@
       <c r="B42" s="10" t="s">
         <v>34</v>
       </c>
+      <c r="C42" s="11">
+        <v>30.123999999999999</v>
+      </c>
+      <c r="D42" s="11">
+        <v>3.7570000000000001</v>
+      </c>
       <c r="F42" s="11">
-        <v>1706.2809999999999</v>
+        <v>1862.93</v>
       </c>
       <c r="G42" s="11">
-        <v>0.77300000000000002</v>
+        <v>27.468</v>
       </c>
       <c r="I42" s="11">
-        <v>1017.0309999999999</v>
+        <v>1119.883</v>
       </c>
       <c r="J42" s="11">
-        <v>1.216</v>
+        <v>18.015999999999998</v>
       </c>
       <c r="L42" s="11">
-        <v>988.84199999999998</v>
+        <v>1229.9749999999999</v>
       </c>
       <c r="M42" s="11">
-        <v>0.91700000000000004</v>
+        <v>18.547000000000001</v>
       </c>
       <c r="O42" s="11">
-        <v>949.875</v>
+        <v>860.68299999999999</v>
       </c>
       <c r="P42" s="11">
-        <v>0.93700000000000006</v>
+        <v>15.789</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -2184,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="11">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="J43" s="11">
         <v>0</v>
@@ -2196,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="O43" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="P43" s="11">
         <v>0</v>
@@ -2207,25 +2211,25 @@
         <v>36</v>
       </c>
       <c r="F44" s="11">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G44" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I44" s="11">
         <v>0.83099999999999996</v>
       </c>
-      <c r="G44" s="11">
-        <v>1E-3</v>
-      </c>
-      <c r="I44" s="11">
-        <v>0.83499999999999996</v>
-      </c>
       <c r="J44" s="11">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="L44" s="11">
         <v>0.81499999999999995</v>
       </c>
       <c r="M44" s="11">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="O44" s="11">
-        <v>0.82299999999999995</v>
+        <v>0.85</v>
       </c>
       <c r="P44" s="11">
         <v>2E-3</v>
@@ -2236,28 +2240,28 @@
         <v>37</v>
       </c>
       <c r="F45" s="11">
-        <v>0.79700000000000004</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="G45" s="11">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="I45" s="11">
-        <v>0.57099999999999995</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="J45" s="11">
-        <v>3.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="L45" s="11">
         <v>0.59399999999999997</v>
       </c>
       <c r="M45" s="11">
-        <v>3.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="O45" s="11">
-        <v>0.66200000000000003</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="P45" s="11">
-        <v>3.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -2265,32 +2269,36 @@
       <c r="B46" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
+      <c r="C46" s="27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D46" s="27">
+        <v>2E-3</v>
+      </c>
       <c r="E46" s="27"/>
       <c r="F46" s="27">
-        <v>5.1999999999999998E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="G46" s="27">
         <v>0</v>
       </c>
       <c r="H46" s="27"/>
       <c r="I46" s="27">
-        <v>4.5999999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="J46" s="27">
         <v>0</v>
       </c>
       <c r="K46" s="27"/>
       <c r="L46" s="27">
-        <v>4.7E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="M46" s="27">
         <v>0</v>
       </c>
       <c r="N46" s="27"/>
       <c r="O46" s="27">
-        <v>4.2999999999999997E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="P46" s="27">
         <v>0</v>
@@ -2302,8 +2310,12 @@
       <c r="B47" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
+      <c r="C47" s="27">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="D47" s="27">
+        <v>8.9999999999999993E-3</v>
+      </c>
       <c r="E47" s="27"/>
       <c r="F47" s="27"/>
       <c r="G47" s="27"/>
@@ -2312,21 +2324,21 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="J47" s="27">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="K47" s="27"/>
       <c r="L47" s="27">
-        <v>7.1999999999999995E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="M47" s="27">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="N47" s="27"/>
       <c r="O47" s="27">
-        <v>0.06</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="P47" s="27">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="Q47" s="27"/>
     </row>
@@ -2335,8 +2347,12 @@
       <c r="B48" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
+      <c r="C48" s="19">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="D48" s="19">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
@@ -2348,10 +2364,10 @@
       <c r="M48" s="19"/>
       <c r="N48" s="19"/>
       <c r="O48" s="19">
-        <v>0.27900000000000003</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="P48" s="19">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="Q48" s="19"/>
     </row>
@@ -2370,7 +2386,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82BA664-5BFD-4584-901E-4E115AE15449}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3138,7 +3154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8880E970-FBCA-47E4-96C7-FF2A26A3D137}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4345,7 +4361,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4998C18F-23F0-496C-92E6-D0C9725AA44B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5549,7 +5565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711747C5-4812-404C-A975-2FE4A1BB38CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6769,7 +6785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8918222-85D2-449B-8A18-73485E61711E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7992,7 +8008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796CB5DF-D73E-45ED-8F43-E9440DD9A3F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9205,7 +9221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB94F20-E3CE-4756-A34F-B261DEC836B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10382,7 +10398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F48C321-BCA3-4D4B-9401-D8A384CBD26D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11585,7 +11601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F878E3BA-8E2E-4762-96F8-C4FCC579D537}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12793,7 +12809,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DD9E6F-5DC3-40EC-B7BB-5197EF2F2C30}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13994,14 +14010,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I38" sqref="I38"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -14795,7 +14811,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="19">
-        <v>3826.22</v>
+        <v>3826.2190000000001</v>
       </c>
       <c r="D34" s="19">
         <v>304.05099999999999</v>
@@ -15101,7 +15117,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896B5996-A248-4FFB-BE2F-226D0C5F7301}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16219,7 +16235,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8F8887-EE9E-4567-BCAF-768E7BCF4F0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17413,7 +17429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE13F8A-181A-4E87-BD2E-529BD8B5AD6D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18622,7 +18638,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8312C19-C14A-4C5D-B16C-3F63EB9485EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19642,7 +19658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8260F7-D0C9-4EC5-A190-C90A3244D50D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20857,7 +20873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AE205F-2DA1-4524-A803-B809E7BA12EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22051,7 +22067,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0FC168-6698-458E-BEAA-5263CC7A0F1F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23261,7 +23277,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C61AF70-8E80-4AE9-86CA-B9954E5AC076}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24510,7 +24526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45D9552-CAB9-4225-A20D-6005283A44DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Update modification indices with MMIed data
</commit_message>
<xml_diff>
--- a/Model building/Results 20.xlsx
+++ b/Model building/Results 20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5032A9AE-EA15-4E53-9B54-52CB3294AFDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A56EE87-E9ED-415F-9F31-582A56B506DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15435" tabRatio="640" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14715" yWindow="4035" windowWidth="15960" windowHeight="10170" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="21" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="71">
   <si>
     <t>Null Model</t>
   </si>
@@ -766,11 +766,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomRight" activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -900,37 +900,37 @@
         <v>5</v>
       </c>
       <c r="F4" s="11">
-        <v>449.92399999999998</v>
+        <v>449.92</v>
       </c>
       <c r="G4" s="11">
-        <v>1.728</v>
+        <v>1.726</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="11">
-        <v>444.23700000000002</v>
+        <v>444.21499999999997</v>
       </c>
       <c r="J4" s="11">
-        <v>2.5960000000000001</v>
+        <v>2.5950000000000002</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="L4" s="11">
-        <v>484.48099999999999</v>
+        <v>484.52</v>
       </c>
       <c r="M4" s="11">
-        <v>4.8419999999999996</v>
+        <v>4.8730000000000002</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O4" s="11">
-        <v>392.88</v>
+        <v>392.90699999999998</v>
       </c>
       <c r="P4" s="11">
-        <v>14.074</v>
+        <v>14.073</v>
       </c>
       <c r="Q4" s="11" t="s">
         <v>5</v>
@@ -971,7 +971,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="11">
-        <v>-0.03</v>
+        <v>-3.1E-2</v>
       </c>
       <c r="J6" s="11">
         <v>1.0999999999999999E-2</v>
@@ -1003,7 +1003,7 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14">
-        <v>-0.125</v>
+        <v>-0.124</v>
       </c>
       <c r="G7" s="14">
         <v>8.0000000000000002E-3</v>
@@ -1047,7 +1047,7 @@
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
       <c r="F8" s="25">
-        <v>5.8000000000000003E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="G8" s="25">
         <v>3.0000000000000001E-3</v>
@@ -1065,7 +1065,7 @@
         <v>5</v>
       </c>
       <c r="L8" s="25">
-        <v>6.0999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="M8" s="25">
         <v>4.0000000000000001E-3</v>
@@ -1091,7 +1091,7 @@
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
       <c r="F9" s="25">
-        <v>5.5E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="G9" s="25">
         <v>3.0000000000000001E-3</v>
@@ -1138,7 +1138,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G10" s="25">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>16</v>
@@ -1176,16 +1176,16 @@
         <v>14</v>
       </c>
       <c r="F11" s="11">
-        <v>7.8E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="G11" s="11">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="11">
-        <v>5.6000000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="J11" s="11">
         <v>8.9999999999999993E-3</v>
@@ -1194,7 +1194,7 @@
         <v>5</v>
       </c>
       <c r="L11" s="11">
-        <v>5.6000000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="M11" s="11">
         <v>8.9999999999999993E-3</v>
@@ -1264,7 +1264,7 @@
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
       <c r="F13" s="25">
-        <v>1.7000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G13" s="25">
         <v>2E-3</v>
@@ -1308,7 +1308,7 @@
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
       <c r="F14" s="25">
-        <v>1.7000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G14" s="25">
         <v>2E-3</v>
@@ -1385,7 +1385,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="11">
-        <v>1.6E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G16" s="11">
         <v>8.0000000000000002E-3</v>
@@ -1400,7 +1400,7 @@
         <v>0.01</v>
       </c>
       <c r="L16" s="11">
-        <v>1.4999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="M16" s="11">
         <v>0.01</v>
@@ -1461,10 +1461,10 @@
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
       <c r="F18" s="25">
-        <v>0.03</v>
+        <v>3.1E-2</v>
       </c>
       <c r="G18" s="25">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H18" s="25" t="s">
         <v>5</v>
@@ -1617,7 +1617,7 @@
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="P21" s="15">
-        <v>1.2999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="Q21" s="11" t="s">
         <v>8</v>
@@ -1652,7 +1652,7 @@
         <v>-2.1000000000000001E-2</v>
       </c>
       <c r="P22" s="15">
-        <v>1.0999999999999999E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="Q22" s="11" t="s">
         <v>9</v>
@@ -1698,7 +1698,7 @@
         <v>69</v>
       </c>
       <c r="F24" s="11">
-        <v>0.44800000000000001</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="G24" s="11">
         <v>8.0000000000000002E-3</v>
@@ -1792,10 +1792,10 @@
         <v>5</v>
       </c>
       <c r="O27" s="11">
-        <v>0.41099999999999998</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="P27" s="11">
-        <v>5.0999999999999997E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="Q27" s="11" t="s">
         <v>5</v>
@@ -1817,10 +1817,13 @@
         <v>5</v>
       </c>
       <c r="O28" s="11">
-        <v>-0.10199999999999999</v>
+        <v>-0.108</v>
       </c>
       <c r="P28" s="11">
         <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="Q28" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1860,7 +1863,7 @@
         <v>5</v>
       </c>
       <c r="O30" s="11">
-        <v>-4.0000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="P30" s="11">
         <v>0.06</v>
@@ -1919,31 +1922,31 @@
       </c>
       <c r="E35" s="27"/>
       <c r="F35" s="27">
-        <v>7789.9570000000003</v>
+        <v>7789.8990000000003</v>
       </c>
       <c r="G35" s="27">
-        <v>111.176</v>
+        <v>111.17</v>
       </c>
       <c r="H35" s="27"/>
       <c r="I35" s="27">
-        <v>5760.9390000000003</v>
+        <v>5760.9350000000004</v>
       </c>
       <c r="J35" s="27">
-        <v>129.51900000000001</v>
+        <v>129.518</v>
       </c>
       <c r="K35" s="27"/>
       <c r="L35" s="27">
-        <v>5760.9690000000001</v>
+        <v>5760.9769999999999</v>
       </c>
       <c r="M35" s="27">
-        <v>129.51499999999999</v>
+        <v>129.51900000000001</v>
       </c>
       <c r="N35" s="27"/>
       <c r="O35" s="27">
-        <v>5742.1440000000002</v>
+        <v>5742.134</v>
       </c>
       <c r="P35" s="27">
-        <v>249.886</v>
+        <v>249.88499999999999</v>
       </c>
       <c r="Q35" s="27"/>
     </row>
@@ -1963,24 +1966,24 @@
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
       <c r="I36" s="27">
-        <v>3251.7449999999999</v>
+        <v>3252.3180000000002</v>
       </c>
       <c r="J36" s="27">
-        <v>195.25800000000001</v>
+        <v>195.28200000000001</v>
       </c>
       <c r="K36" s="27"/>
       <c r="L36" s="27">
-        <v>1621.6949999999999</v>
+        <v>1614.2449999999999</v>
       </c>
       <c r="M36" s="27">
-        <v>142.679</v>
+        <v>143.56399999999999</v>
       </c>
       <c r="N36" s="27"/>
       <c r="O36" s="27">
-        <v>1064.1089999999999</v>
+        <v>1065.759</v>
       </c>
       <c r="P36" s="27">
-        <v>130.85400000000001</v>
+        <v>131.495</v>
       </c>
       <c r="Q36" s="27"/>
     </row>
@@ -2006,10 +2009,10 @@
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
       <c r="O37" s="19">
-        <v>715.69200000000001</v>
+        <v>715.41</v>
       </c>
       <c r="P37" s="19">
-        <v>211.94499999999999</v>
+        <v>211.88499999999999</v>
       </c>
       <c r="Q37" s="19"/>
     </row>
@@ -2071,31 +2074,31 @@
       </c>
       <c r="E40" s="23"/>
       <c r="F40" s="23">
-        <v>3516405.7230000002</v>
+        <v>3428325.0959999999</v>
       </c>
       <c r="G40" s="23">
-        <v>1347.971</v>
+        <v>1724.2909999999999</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23">
-        <v>3539126.6170000001</v>
+        <v>3467536.6469999999</v>
       </c>
       <c r="J40" s="23">
-        <v>1692.1510000000001</v>
+        <v>2082.5210000000002</v>
       </c>
       <c r="K40" s="23"/>
       <c r="L40" s="23">
-        <v>3497150.173</v>
+        <v>3425559.9890000001</v>
       </c>
       <c r="M40" s="23">
-        <v>1608.317</v>
+        <v>2005.96</v>
       </c>
       <c r="N40" s="23"/>
       <c r="O40" s="23">
-        <v>3886028.93</v>
+        <v>3775763.693</v>
       </c>
       <c r="P40" s="23">
-        <v>616.88</v>
+        <v>845.58699999999999</v>
       </c>
       <c r="Q40" s="23"/>
     </row>
@@ -2112,31 +2115,31 @@
       </c>
       <c r="E41" s="23"/>
       <c r="F41" s="23">
-        <v>3516750.6779999998</v>
+        <v>3428813.7829999998</v>
       </c>
       <c r="G41" s="23">
-        <v>1347.971</v>
+        <v>1724.2909999999999</v>
       </c>
       <c r="H41" s="23"/>
       <c r="I41" s="23">
-        <v>3539672.7960000001</v>
+        <v>3468159.483</v>
       </c>
       <c r="J41" s="23">
-        <v>1592.1510000000001</v>
+        <v>2082.5210000000002</v>
       </c>
       <c r="K41" s="23"/>
       <c r="L41" s="23">
-        <v>3497638.86</v>
+        <v>3426125</v>
       </c>
       <c r="M41" s="23">
-        <v>1608.317</v>
+        <v>332</v>
       </c>
       <c r="N41" s="23"/>
       <c r="O41" s="23">
-        <v>3886572.1770000001</v>
+        <v>3776384.5469999998</v>
       </c>
       <c r="P41" s="23">
-        <v>616.88</v>
+        <v>845.58699999999999</v>
       </c>
       <c r="Q41" s="23"/>
     </row>
@@ -2151,28 +2154,28 @@
         <v>3.7570000000000001</v>
       </c>
       <c r="F42" s="11">
-        <v>1862.93</v>
+        <v>1406.588</v>
       </c>
       <c r="G42" s="11">
-        <v>27.468</v>
+        <v>21.396999999999998</v>
       </c>
       <c r="I42" s="11">
-        <v>1119.883</v>
+        <v>1027.934</v>
       </c>
       <c r="J42" s="11">
-        <v>18.015999999999998</v>
+        <v>18.041</v>
       </c>
       <c r="L42" s="11">
-        <v>1229.9749999999999</v>
+        <v>1121.4739999999999</v>
       </c>
       <c r="M42" s="11">
-        <v>18.547000000000001</v>
+        <v>18.544</v>
       </c>
       <c r="O42" s="11">
-        <v>860.68299999999999</v>
+        <v>2390.4</v>
       </c>
       <c r="P42" s="11">
-        <v>15.789</v>
+        <v>114.06399999999999</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -2180,28 +2183,28 @@
         <v>34</v>
       </c>
       <c r="F43" s="11">
-        <v>2.9000000000000001E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="G43" s="11">
         <v>0</v>
       </c>
       <c r="I43" s="11">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="J43" s="11">
         <v>0</v>
       </c>
       <c r="L43" s="11">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="M43" s="11">
         <v>0</v>
       </c>
       <c r="O43" s="11">
-        <v>1.4999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="P43" s="11">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -2209,28 +2212,28 @@
         <v>35</v>
       </c>
       <c r="F44" s="11">
-        <v>0.82699999999999996</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="G44" s="11">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="I44" s="11">
-        <v>0.83099999999999996</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="J44" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="L44" s="11">
-        <v>0.81499999999999995</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="M44" s="11">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="O44" s="11">
-        <v>0.85</v>
+        <v>0.995</v>
       </c>
       <c r="P44" s="11">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -2238,28 +2241,28 @@
         <v>36</v>
       </c>
       <c r="F45" s="11">
-        <v>0.79200000000000004</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="G45" s="11">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I45" s="11">
-        <v>0.56299999999999994</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="J45" s="11">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="L45" s="11">
-        <v>0.59399999999999997</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="M45" s="11">
-        <v>7.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="O45" s="11">
-        <v>0.71299999999999997</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="P45" s="11">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -2275,28 +2278,28 @@
       </c>
       <c r="E46" s="27"/>
       <c r="F46" s="27">
-        <v>5.0999999999999997E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="G46" s="27">
         <v>0</v>
       </c>
       <c r="H46" s="27"/>
       <c r="I46" s="27">
-        <v>4.4999999999999998E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="J46" s="27">
         <v>0</v>
       </c>
       <c r="K46" s="27"/>
       <c r="L46" s="27">
-        <v>4.4999999999999998E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M46" s="27">
         <v>0</v>
       </c>
       <c r="N46" s="27"/>
       <c r="O46" s="27">
-        <v>4.2000000000000003E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="P46" s="27">
         <v>0</v>
@@ -2319,21 +2322,21 @@
       <c r="G47" s="27"/>
       <c r="H47" s="27"/>
       <c r="I47" s="27">
-        <v>6.8000000000000005E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="J47" s="27">
         <v>2E-3</v>
       </c>
       <c r="K47" s="27"/>
       <c r="L47" s="27">
-        <v>7.2999999999999995E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="M47" s="27">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="N47" s="27"/>
       <c r="O47" s="27">
-        <v>5.8999999999999997E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="P47" s="27">
         <v>2E-3</v>
@@ -2362,7 +2365,7 @@
       <c r="M48" s="19"/>
       <c r="N48" s="19"/>
       <c r="O48" s="19">
-        <v>0.27400000000000002</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="P48" s="19">
         <v>2E-3</v>
@@ -16269,7 +16272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F10" sqref="F10"/>
       <selection pane="topRight" activeCell="F10" sqref="F10"/>

</xml_diff>

<commit_message>
Update models with fresh multilevel MI datasets
</commit_message>
<xml_diff>
--- a/Model building/Results 20.xlsx
+++ b/Model building/Results 20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A56EE87-E9ED-415F-9F31-582A56B506DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D698F27-91B3-4C51-97DE-7EBD73C35827}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14715" yWindow="4035" windowWidth="15960" windowHeight="10170" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="71">
   <si>
     <t>Null Model</t>
   </si>
@@ -770,7 +770,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O32" sqref="O32"/>
+      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -900,37 +900,37 @@
         <v>5</v>
       </c>
       <c r="F4" s="11">
-        <v>449.92</v>
+        <v>450.03399999999999</v>
       </c>
       <c r="G4" s="11">
-        <v>1.726</v>
+        <v>1.7310000000000001</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="11">
-        <v>444.21499999999997</v>
+        <v>444.29199999999997</v>
       </c>
       <c r="J4" s="11">
-        <v>2.5950000000000002</v>
+        <v>2.6120000000000001</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="L4" s="11">
-        <v>484.52</v>
+        <v>485.82900000000001</v>
       </c>
       <c r="M4" s="11">
-        <v>4.8730000000000002</v>
+        <v>138.785</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O4" s="11">
-        <v>392.90699999999998</v>
+        <v>392.52</v>
       </c>
       <c r="P4" s="11">
-        <v>14.073</v>
+        <v>14.002000000000001</v>
       </c>
       <c r="Q4" s="11" t="s">
         <v>5</v>
@@ -962,16 +962,16 @@
         <v>7</v>
       </c>
       <c r="F6" s="11">
-        <v>-6.7000000000000004E-2</v>
+        <v>-6.8000000000000005E-2</v>
       </c>
       <c r="G6" s="11">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="11">
-        <v>-3.1E-2</v>
+        <v>-3.2000000000000001E-2</v>
       </c>
       <c r="J6" s="11">
         <v>1.0999999999999999E-2</v>
@@ -980,7 +980,7 @@
         <v>8</v>
       </c>
       <c r="L6" s="11">
-        <v>-0.03</v>
+        <v>-3.1E-2</v>
       </c>
       <c r="M6" s="11">
         <v>1.0999999999999999E-2</v>
@@ -989,10 +989,10 @@
         <v>8</v>
       </c>
       <c r="O6" s="11">
-        <v>-6.0000000000000001E-3</v>
+        <v>-8.9999999999999993E-3</v>
       </c>
       <c r="P6" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1003,7 +1003,7 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14">
-        <v>-0.124</v>
+        <v>-0.125</v>
       </c>
       <c r="G7" s="14">
         <v>8.0000000000000002E-3</v>
@@ -1012,7 +1012,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="14">
-        <v>-0.09</v>
+        <v>-9.0999999999999998E-2</v>
       </c>
       <c r="J7" s="14">
         <v>1.0999999999999999E-2</v>
@@ -1021,7 +1021,7 @@
         <v>5</v>
       </c>
       <c r="L7" s="14">
-        <v>-0.09</v>
+        <v>-9.0999999999999998E-2</v>
       </c>
       <c r="M7" s="14">
         <v>1.0999999999999999E-2</v>
@@ -1030,10 +1030,10 @@
         <v>5</v>
       </c>
       <c r="O7" s="14">
-        <v>-7.3999999999999996E-2</v>
+        <v>-7.5999999999999998E-2</v>
       </c>
       <c r="P7" s="14">
-        <v>1.4999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="Q7" s="14" t="s">
         <v>5</v>
@@ -1056,7 +1056,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="25">
-        <v>0.06</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="J8" s="25">
         <v>4.0000000000000001E-3</v>
@@ -1065,7 +1065,7 @@
         <v>5</v>
       </c>
       <c r="L8" s="25">
-        <v>0.06</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="M8" s="25">
         <v>4.0000000000000001E-3</v>
@@ -1074,7 +1074,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="25">
-        <v>6.8000000000000005E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="P8" s="25">
         <v>5.0000000000000001E-3</v>
@@ -1138,7 +1138,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G10" s="25">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>16</v>
@@ -1162,7 +1162,7 @@
         <v>5</v>
       </c>
       <c r="O10" s="25">
-        <v>1.0999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="P10" s="25">
         <v>2E-3</v>
@@ -1176,7 +1176,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="11">
-        <v>7.9000000000000001E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="G11" s="11">
         <v>7.0000000000000001E-3</v>
@@ -1203,7 +1203,7 @@
         <v>5</v>
       </c>
       <c r="O11" s="11">
-        <v>6.8000000000000005E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="P11" s="11">
         <v>7.0000000000000001E-3</v>
@@ -1220,7 +1220,7 @@
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14">
-        <v>6.0999999999999999E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G12" s="14">
         <v>7.0000000000000001E-3</v>
@@ -1229,7 +1229,7 @@
         <v>5</v>
       </c>
       <c r="I12" s="14">
-        <v>4.5999999999999999E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="J12" s="14">
         <v>8.9999999999999993E-3</v>
@@ -1238,7 +1238,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="14">
-        <v>4.5999999999999999E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="M12" s="14">
         <v>8.9999999999999993E-3</v>
@@ -1250,7 +1250,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="P12" s="14">
-        <v>6.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="Q12" s="14" t="s">
         <v>5</v>
@@ -1264,7 +1264,7 @@
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
       <c r="F13" s="25">
-        <v>1.7999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G13" s="25">
         <v>2E-3</v>
@@ -1291,7 +1291,7 @@
         <v>5</v>
       </c>
       <c r="O13" s="25">
-        <v>1.2E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="P13" s="25">
         <v>1E-3</v>
@@ -1308,7 +1308,7 @@
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
       <c r="F14" s="25">
-        <v>1.7999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G14" s="25">
         <v>2E-3</v>
@@ -1373,12 +1373,14 @@
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="25">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="P15" s="25">
         <v>1E-3</v>
       </c>
-      <c r="Q15" s="25"/>
+      <c r="Q15" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
@@ -1388,13 +1390,13 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="G16" s="11">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>9</v>
       </c>
       <c r="I16" s="11">
-        <v>1.6E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="J16" s="11">
         <v>0.01</v>
@@ -1406,7 +1408,7 @@
         <v>0.01</v>
       </c>
       <c r="O16" s="11">
-        <v>0.03</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="P16" s="11">
         <v>1.2999999999999999E-2</v>
@@ -1435,21 +1437,21 @@
         <v>-1.4E-2</v>
       </c>
       <c r="J17" s="14">
-        <v>8.9999999999999993E-3</v>
+        <v>0.01</v>
       </c>
       <c r="K17" s="14"/>
       <c r="L17" s="14">
         <v>-1.4E-2</v>
       </c>
       <c r="M17" s="14">
-        <v>8.9999999999999993E-3</v>
+        <v>0.01</v>
       </c>
       <c r="N17" s="14"/>
       <c r="O17" s="14">
-        <v>-5.0000000000000001E-3</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="P17" s="14">
-        <v>1.2E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="Q17" s="14"/>
     </row>
@@ -1464,7 +1466,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="G18" s="25">
-        <v>3.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="H18" s="25" t="s">
         <v>5</v>
@@ -1488,7 +1490,7 @@
         <v>5</v>
       </c>
       <c r="O18" s="25">
-        <v>3.4000000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="P18" s="25">
         <v>3.0000000000000001E-3</v>
@@ -1514,7 +1516,7 @@
         <v>5</v>
       </c>
       <c r="I19" s="25">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="J19" s="25">
         <v>2E-3</v>
@@ -1576,7 +1578,7 @@
         <v>8</v>
       </c>
       <c r="O20" s="25">
-        <v>0.01</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="P20" s="25">
         <v>2E-3</v>
@@ -1596,7 +1598,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="I21" s="15">
-        <v>-3.7999999999999999E-2</v>
+        <v>-3.9E-2</v>
       </c>
       <c r="J21" s="15">
         <v>1.2E-2</v>
@@ -1605,7 +1607,7 @@
         <v>8</v>
       </c>
       <c r="L21" s="15">
-        <v>-3.7999999999999999E-2</v>
+        <v>-3.9E-2</v>
       </c>
       <c r="M21" s="15">
         <v>1.2E-2</v>
@@ -1640,13 +1642,13 @@
         <v>1.6E-2</v>
       </c>
       <c r="J22" s="15">
-        <v>1.2E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="L22" s="15">
         <v>1.6E-2</v>
       </c>
       <c r="M22" s="15">
-        <v>1.2E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="O22" s="15">
         <v>-2.1000000000000001E-2</v>
@@ -1684,7 +1686,7 @@
         <v>0.01</v>
       </c>
       <c r="O23" s="11">
-        <v>1.9E-2</v>
+        <v>0.02</v>
       </c>
       <c r="P23" s="11">
         <v>1.0999999999999999E-2</v>
@@ -1701,31 +1703,31 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="G24" s="11">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="11">
-        <v>0.245</v>
+        <v>0.246</v>
       </c>
       <c r="J24" s="11">
-        <v>1.6E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="L24" s="11">
-        <v>0.245</v>
+        <v>0.246</v>
       </c>
       <c r="M24" s="11">
-        <v>1.6E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="N24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O24" s="11">
-        <v>0.19400000000000001</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="P24" s="11">
         <v>1.7000000000000001E-2</v>
@@ -1760,19 +1762,19 @@
         <v>21</v>
       </c>
       <c r="L26" s="11">
-        <v>-0.27900000000000003</v>
+        <v>-0.26800000000000002</v>
       </c>
       <c r="M26" s="11">
-        <v>5.3999999999999999E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="N26" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O26" s="11">
-        <v>-0.27900000000000003</v>
+        <v>-0.28799999999999998</v>
       </c>
       <c r="P26" s="11">
-        <v>5.8999999999999997E-2</v>
+        <v>0.06</v>
       </c>
       <c r="Q26" s="11" t="s">
         <v>5</v>
@@ -1783,19 +1785,19 @@
         <v>22</v>
       </c>
       <c r="L27" s="11">
-        <v>0.20499999999999999</v>
+        <v>0.249</v>
       </c>
       <c r="M27" s="11">
-        <v>5.8000000000000003E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="N27" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O27" s="11">
-        <v>0.40600000000000003</v>
+        <v>0.41</v>
       </c>
       <c r="P27" s="11">
-        <v>5.1999999999999998E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="Q27" s="11" t="s">
         <v>5</v>
@@ -1808,7 +1810,7 @@
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="L28" s="11">
-        <v>-0.27500000000000002</v>
+        <v>-0.29199999999999998</v>
       </c>
       <c r="M28" s="11">
         <v>5.3999999999999999E-2</v>
@@ -1817,10 +1819,10 @@
         <v>5</v>
       </c>
       <c r="O28" s="11">
-        <v>-0.108</v>
+        <v>-0.10100000000000001</v>
       </c>
       <c r="P28" s="11">
-        <v>5.8000000000000003E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="Q28" s="11" t="s">
         <v>16</v>
@@ -1831,10 +1833,10 @@
         <v>24</v>
       </c>
       <c r="L29" s="11">
-        <v>-0.28399999999999997</v>
+        <v>-0.26700000000000002</v>
       </c>
       <c r="M29" s="11">
-        <v>3.6999999999999998E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="N29" s="11" t="s">
         <v>5</v>
@@ -1843,7 +1845,7 @@
         <v>-0.157</v>
       </c>
       <c r="P29" s="11">
-        <v>3.5999999999999997E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="Q29" s="11" t="s">
         <v>5</v>
@@ -1854,19 +1856,19 @@
         <v>25</v>
       </c>
       <c r="L30" s="11">
-        <v>-0.111</v>
+        <v>-0.122</v>
       </c>
       <c r="M30" s="11">
-        <v>2.8000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="N30" s="11" t="s">
         <v>5</v>
       </c>
       <c r="O30" s="11">
-        <v>-5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="P30" s="11">
-        <v>0.06</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1922,31 +1924,31 @@
       </c>
       <c r="E35" s="27"/>
       <c r="F35" s="27">
-        <v>7789.8990000000003</v>
+        <v>7785.2370000000001</v>
       </c>
       <c r="G35" s="27">
-        <v>111.17</v>
+        <v>109.813</v>
       </c>
       <c r="H35" s="27"/>
       <c r="I35" s="27">
-        <v>5760.9350000000004</v>
+        <v>5759.3490000000002</v>
       </c>
       <c r="J35" s="27">
-        <v>129.518</v>
+        <v>130.28899999999999</v>
       </c>
       <c r="K35" s="27"/>
       <c r="L35" s="27">
-        <v>5760.9769999999999</v>
+        <v>5759.3909999999996</v>
       </c>
       <c r="M35" s="27">
-        <v>129.51900000000001</v>
+        <v>130.291</v>
       </c>
       <c r="N35" s="27"/>
       <c r="O35" s="27">
-        <v>5742.134</v>
+        <v>5740.3789999999999</v>
       </c>
       <c r="P35" s="27">
-        <v>249.88499999999999</v>
+        <v>250.01599999999999</v>
       </c>
       <c r="Q35" s="27"/>
     </row>
@@ -1966,24 +1968,24 @@
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
       <c r="I36" s="27">
-        <v>3252.3180000000002</v>
+        <v>3252.1379999999999</v>
       </c>
       <c r="J36" s="27">
-        <v>195.28200000000001</v>
+        <v>194.482</v>
       </c>
       <c r="K36" s="27"/>
       <c r="L36" s="27">
-        <v>1614.2449999999999</v>
+        <v>1560.6320000000001</v>
       </c>
       <c r="M36" s="27">
-        <v>143.56399999999999</v>
+        <v>138.785</v>
       </c>
       <c r="N36" s="27"/>
       <c r="O36" s="27">
-        <v>1065.759</v>
+        <v>1050.8030000000001</v>
       </c>
       <c r="P36" s="27">
-        <v>131.495</v>
+        <v>128.56100000000001</v>
       </c>
       <c r="Q36" s="27"/>
     </row>
@@ -2009,10 +2011,10 @@
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
       <c r="O37" s="19">
-        <v>715.41</v>
+        <v>716.87</v>
       </c>
       <c r="P37" s="19">
-        <v>211.88499999999999</v>
+        <v>211.93</v>
       </c>
       <c r="Q37" s="19"/>
     </row>
@@ -2074,31 +2076,31 @@
       </c>
       <c r="E40" s="23"/>
       <c r="F40" s="23">
-        <v>3428325.0959999999</v>
+        <v>3428037.7250000001</v>
       </c>
       <c r="G40" s="23">
-        <v>1724.2909999999999</v>
+        <v>1185.779</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23">
-        <v>3467536.6469999999</v>
+        <v>3467032.4440000001</v>
       </c>
       <c r="J40" s="23">
-        <v>2082.5210000000002</v>
+        <v>1188.77</v>
       </c>
       <c r="K40" s="23"/>
       <c r="L40" s="23">
-        <v>3425559.9890000001</v>
+        <v>3425082.9739999999</v>
       </c>
       <c r="M40" s="23">
-        <v>2005.96</v>
+        <v>1180.6759999999999</v>
       </c>
       <c r="N40" s="23"/>
       <c r="O40" s="23">
-        <v>3775763.693</v>
+        <v>3775486.2390000001</v>
       </c>
       <c r="P40" s="23">
-        <v>845.58699999999999</v>
+        <v>983.43600000000004</v>
       </c>
       <c r="Q40" s="23"/>
     </row>
@@ -2115,31 +2117,31 @@
       </c>
       <c r="E41" s="23"/>
       <c r="F41" s="23">
-        <v>3428813.7829999998</v>
+        <v>3428526.412</v>
       </c>
       <c r="G41" s="23">
-        <v>1724.2909999999999</v>
+        <v>1185.779</v>
       </c>
       <c r="H41" s="23"/>
       <c r="I41" s="23">
-        <v>3468159.483</v>
+        <v>3467655.281</v>
       </c>
       <c r="J41" s="23">
-        <v>2082.5210000000002</v>
+        <v>1188.77</v>
       </c>
       <c r="K41" s="23"/>
       <c r="L41" s="23">
-        <v>3426125</v>
+        <v>3425648.318</v>
       </c>
       <c r="M41" s="23">
-        <v>332</v>
+        <v>1180.6759999999999</v>
       </c>
       <c r="N41" s="23"/>
       <c r="O41" s="23">
-        <v>3776384.5469999998</v>
+        <v>3776107.0929999999</v>
       </c>
       <c r="P41" s="23">
-        <v>845.58699999999999</v>
+        <v>983.43600000000004</v>
       </c>
       <c r="Q41" s="23"/>
     </row>
@@ -2154,34 +2156,40 @@
         <v>3.7570000000000001</v>
       </c>
       <c r="F42" s="11">
-        <v>1406.588</v>
+        <v>1395.8009999999999</v>
       </c>
       <c r="G42" s="11">
-        <v>21.396999999999998</v>
+        <v>21.984000000000002</v>
       </c>
       <c r="I42" s="11">
-        <v>1027.934</v>
+        <v>1009.82</v>
       </c>
       <c r="J42" s="11">
-        <v>18.041</v>
+        <v>18.335000000000001</v>
       </c>
       <c r="L42" s="11">
-        <v>1121.4739999999999</v>
+        <v>1097.171</v>
       </c>
       <c r="M42" s="11">
-        <v>18.544</v>
+        <v>22.314</v>
       </c>
       <c r="O42" s="11">
-        <v>2390.4</v>
+        <v>2363.0189999999998</v>
       </c>
       <c r="P42" s="11">
-        <v>114.06399999999999</v>
+        <v>84.435000000000002</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
         <v>34</v>
       </c>
+      <c r="C43" s="11">
+        <v>0</v>
+      </c>
+      <c r="D43" s="11">
+        <v>0</v>
+      </c>
       <c r="F43" s="11">
         <v>3.3000000000000002E-2</v>
       </c>
@@ -2204,27 +2212,33 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="P43" s="11">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="C44" s="11">
+        <v>0</v>
+      </c>
+      <c r="D44" s="11">
+        <v>0</v>
+      </c>
       <c r="F44" s="11">
-        <v>0.86899999999999999</v>
+        <v>0.87</v>
       </c>
       <c r="G44" s="11">
+        <v>1E-3</v>
+      </c>
+      <c r="I44" s="11">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="J44" s="11">
         <v>2E-3</v>
       </c>
-      <c r="I44" s="11">
-        <v>0.84799999999999998</v>
-      </c>
-      <c r="J44" s="11">
-        <v>3.0000000000000001E-3</v>
-      </c>
       <c r="L44" s="11">
-        <v>0.83499999999999996</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="M44" s="11">
         <v>2E-3</v>
@@ -2240,29 +2254,35 @@
       <c r="B45" s="10" t="s">
         <v>36</v>
       </c>
+      <c r="C45" s="11">
+        <v>1</v>
+      </c>
+      <c r="D45" s="11">
+        <v>0</v>
+      </c>
       <c r="F45" s="11">
-        <v>0.73699999999999999</v>
+        <v>0.74</v>
       </c>
       <c r="G45" s="11">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="I45" s="11">
-        <v>0.56599999999999995</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="J45" s="11">
-        <v>7.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="L45" s="11">
-        <v>0.60299999999999998</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="M45" s="11">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O45" s="11">
         <v>0.98899999999999999</v>
       </c>
       <c r="P45" s="11">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -2322,24 +2342,24 @@
       <c r="G47" s="27"/>
       <c r="H47" s="27"/>
       <c r="I47" s="27">
-        <v>6.6000000000000003E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="J47" s="27">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K47" s="27"/>
       <c r="L47" s="27">
-        <v>7.1999999999999995E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="M47" s="27">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="N47" s="27"/>
       <c r="O47" s="27">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="P47" s="27">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="Q47" s="27"/>
     </row>
@@ -2368,7 +2388,7 @@
         <v>0.26100000000000001</v>
       </c>
       <c r="P48" s="19">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="Q48" s="19"/>
     </row>

</xml_diff>

<commit_message>
Correct model equations to include intercepts
</commit_message>
<xml_diff>
--- a/Model building/Results 20.xlsx
+++ b/Model building/Results 20.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412EFF78-26B9-4DC7-AA39-E32F550C0ED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="640"/>
   </bookViews>
   <sheets>
     <sheet name="Model Development" sheetId="21" r:id="rId1"/>
     <sheet name="Final" sheetId="22" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="103">
   <si>
     <t>Null Model</t>
   </si>
@@ -147,21 +146,6 @@
       </rPr>
       <t>(residual variances of FLIT)</t>
     </r>
-  </si>
-  <si>
-    <t>Three-level Model</t>
-  </si>
-  <si>
-    <t>Country-level</t>
-  </si>
-  <si>
-    <t>SRMR L3</t>
-  </si>
-  <si>
-    <t>Country-level Predictors</t>
-  </si>
-  <si>
-    <t>FKI</t>
   </si>
   <si>
     <t>76 BRA</t>
@@ -365,7 +349,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -571,9 +555,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -642,10 +623,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -931,48 +915,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="9" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="48" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="47" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="10"/>
-    <col min="5" max="5" width="7.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" style="38" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="37" customWidth="1"/>
     <col min="7" max="7" width="9" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" style="38" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" style="37" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" style="38" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" style="37" customWidth="1"/>
     <col min="13" max="13" width="9" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" style="38" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.42578125" style="38" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="54"/>
+    <col min="15" max="15" width="4.42578125" style="37" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>75</v>
+        <v>58</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>70</v>
       </c>
       <c r="D1" s="60" t="s">
         <v>0</v>
@@ -994,17 +975,12 @@
       </c>
       <c r="N1" s="60"/>
       <c r="O1" s="60"/>
-      <c r="P1" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="46" t="s">
-        <v>74</v>
+      <c r="C2" s="45" t="s">
+        <v>69</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>1</v>
@@ -1012,42 +988,35 @@
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="37"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="37"/>
+      <c r="I2" s="36"/>
       <c r="J2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="37"/>
+      <c r="L2" s="36"/>
       <c r="M2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="37"/>
+      <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="47"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="31"/>
@@ -1060,21 +1029,18 @@
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="31"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="31"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="10">
-        <v>506.27600000000001</v>
+        <v>454.154</v>
       </c>
       <c r="E4" s="10">
-        <v>12.161</v>
-      </c>
-      <c r="F4" s="38" t="s">
+        <v>2.69</v>
+      </c>
+      <c r="F4" s="37" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="10">
@@ -1083,7 +1049,7 @@
       <c r="H4" s="10">
         <v>1.431</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="37" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="10">
@@ -1092,7 +1058,7 @@
       <c r="K4" s="10">
         <v>2.5550000000000002</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="37" t="s">
         <v>5</v>
       </c>
       <c r="M4" s="10">
@@ -1101,25 +1067,16 @@
       <c r="N4" s="10">
         <v>4.7949999999999999</v>
       </c>
-      <c r="O4" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P4" s="10">
-        <v>394.70699999999999</v>
-      </c>
-      <c r="Q4" s="10">
-        <v>14.105</v>
-      </c>
-      <c r="R4" s="38" t="s">
+      <c r="O4" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="49"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="16"/>
@@ -1132,16 +1089,13 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>98</v>
+      <c r="C6" s="47" t="s">
+        <v>93</v>
       </c>
       <c r="G6" s="10">
         <v>-6.8000000000000005E-2</v>
@@ -1149,7 +1103,7 @@
       <c r="H6" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="37" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="10">
@@ -1158,7 +1112,7 @@
       <c r="K6" s="10">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="37" t="s">
         <v>8</v>
       </c>
       <c r="M6" s="10">
@@ -1167,33 +1121,27 @@
       <c r="N6" s="10">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="O6" s="38" t="s">
+      <c r="O6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="10">
-        <v>-8.9999999999999993E-3</v>
-      </c>
-      <c r="Q6" s="10">
-        <v>1.6E-2</v>
-      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
-        <v>70</v>
+      <c r="C7" s="54" t="s">
+        <v>65</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
-      <c r="F7" s="39"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="13">
         <v>-0.126</v>
       </c>
       <c r="H7" s="13">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I7" s="39" t="s">
+      <c r="I7" s="38" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="13">
@@ -1202,7 +1150,7 @@
       <c r="K7" s="13">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="38" t="s">
         <v>5</v>
       </c>
       <c r="M7" s="13">
@@ -1211,36 +1159,27 @@
       <c r="N7" s="13">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="O7" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="P7" s="13">
-        <v>-7.4999999999999997E-2</v>
-      </c>
-      <c r="Q7" s="13">
-        <v>1.4E-2</v>
-      </c>
-      <c r="R7" s="39" t="s">
+      <c r="O7" s="38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>97</v>
+      <c r="C8" s="49" t="s">
+        <v>92</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="40"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="24">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="H8" s="24">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="39" t="s">
         <v>5</v>
       </c>
       <c r="J8" s="24">
@@ -1249,7 +1188,7 @@
       <c r="K8" s="24">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L8" s="40" t="s">
+      <c r="L8" s="39" t="s">
         <v>5</v>
       </c>
       <c r="M8" s="24">
@@ -1258,36 +1197,27 @@
       <c r="N8" s="24">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O8" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="24">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="Q8" s="24">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="R8" s="40" t="s">
+      <c r="O8" s="39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B9" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>76</v>
+        <v>63</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>71</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="40"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="24">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="H9" s="24">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="39" t="s">
         <v>5</v>
       </c>
       <c r="J9" s="24">
@@ -1296,7 +1226,7 @@
       <c r="K9" s="24">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L9" s="40" t="s">
+      <c r="L9" s="39" t="s">
         <v>5</v>
       </c>
       <c r="M9" s="24">
@@ -1305,43 +1235,34 @@
       <c r="N9" s="24">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O9" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="P9" s="24">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="Q9" s="24">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="R9" s="40" t="s">
+      <c r="O9" s="39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>77</v>
+        <v>64</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>72</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
-      <c r="F10" s="40"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="24">
         <v>2E-3</v>
       </c>
       <c r="H10" s="24">
         <v>2E-3</v>
       </c>
-      <c r="I10" s="40"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="24">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="K10" s="24">
         <v>2E-3</v>
       </c>
-      <c r="L10" s="40" t="s">
+      <c r="L10" s="39" t="s">
         <v>8</v>
       </c>
       <c r="M10" s="24">
@@ -1350,25 +1271,16 @@
       <c r="N10" s="24">
         <v>2E-3</v>
       </c>
-      <c r="O10" s="40" t="s">
+      <c r="O10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="24">
-        <v>0.01</v>
-      </c>
-      <c r="Q10" s="24">
-        <v>2E-3</v>
-      </c>
-      <c r="R10" s="40" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="48" t="s">
-        <v>96</v>
+      <c r="C11" s="47" t="s">
+        <v>91</v>
       </c>
       <c r="G11" s="10">
         <v>1.2999999999999999E-2</v>
@@ -1377,7 +1289,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J11" s="10">
         <v>8.9999999999999993E-3</v>
@@ -1391,33 +1303,24 @@
       <c r="N11" s="10">
         <v>0.01</v>
       </c>
-      <c r="P11" s="10">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="Q11" s="10">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="R11" s="10" t="s">
-        <v>100</v>
-      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="55" t="s">
-        <v>71</v>
+      <c r="C12" s="54" t="s">
+        <v>66</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="39"/>
+      <c r="F12" s="38"/>
       <c r="G12" s="13">
         <v>-1.2E-2</v>
       </c>
       <c r="H12" s="13">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I12" s="39"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="13">
         <v>-1.6E-2</v>
       </c>
@@ -1425,7 +1328,7 @@
         <v>0.01</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M12" s="13">
         <v>-1.6E-2</v>
@@ -1434,33 +1337,26 @@
         <v>0.01</v>
       </c>
       <c r="O12" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="P12" s="13">
-        <v>-6.0000000000000001E-3</v>
-      </c>
-      <c r="Q12" s="13">
-        <v>1.2E-2</v>
-      </c>
-      <c r="R12" s="39"/>
+        <v>95</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B13" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="50" t="s">
-        <v>95</v>
+      <c r="C13" s="49" t="s">
+        <v>90</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="40"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="24">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="H13" s="24">
         <v>2E-3</v>
       </c>
-      <c r="I13" s="40" t="s">
+      <c r="I13" s="39" t="s">
         <v>5</v>
       </c>
       <c r="J13" s="24">
@@ -1469,7 +1365,7 @@
       <c r="K13" s="24">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L13" s="40" t="s">
+      <c r="L13" s="39" t="s">
         <v>5</v>
       </c>
       <c r="M13" s="24">
@@ -1478,36 +1374,27 @@
       <c r="N13" s="24">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O13" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="P13" s="24">
-        <v>3.1E-2</v>
-      </c>
-      <c r="Q13" s="24">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="R13" s="40" t="s">
+      <c r="O13" s="39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>78</v>
+        <v>63</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>73</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
-      <c r="F14" s="40"/>
+      <c r="F14" s="39"/>
       <c r="G14" s="24">
         <v>2.3E-2</v>
       </c>
       <c r="H14" s="24">
         <v>2E-3</v>
       </c>
-      <c r="I14" s="40" t="s">
+      <c r="I14" s="39" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="24">
@@ -1516,7 +1403,7 @@
       <c r="K14" s="24">
         <v>2E-3</v>
       </c>
-      <c r="L14" s="40" t="s">
+      <c r="L14" s="39" t="s">
         <v>5</v>
       </c>
       <c r="M14" s="24">
@@ -1525,43 +1412,34 @@
       <c r="N14" s="24">
         <v>2E-3</v>
       </c>
-      <c r="O14" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="P14" s="24">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="Q14" s="24">
-        <v>2E-3</v>
-      </c>
-      <c r="R14" s="40" t="s">
+      <c r="O14" s="39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>79</v>
+        <v>64</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>74</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="40"/>
+      <c r="F15" s="39"/>
       <c r="G15" s="24">
         <v>2E-3</v>
       </c>
       <c r="H15" s="24">
         <v>1E-3</v>
       </c>
-      <c r="I15" s="40"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="24">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="K15" s="24">
         <v>2E-3</v>
       </c>
-      <c r="L15" s="40" t="s">
+      <c r="L15" s="39" t="s">
         <v>8</v>
       </c>
       <c r="M15" s="24">
@@ -1570,25 +1448,16 @@
       <c r="N15" s="24">
         <v>2E-3</v>
       </c>
-      <c r="O15" s="40" t="s">
+      <c r="O15" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="P15" s="24">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="Q15" s="24">
-        <v>1E-3</v>
-      </c>
-      <c r="R15" s="40" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="56" t="s">
-        <v>94</v>
+      <c r="C16" s="55" t="s">
+        <v>89</v>
       </c>
       <c r="G16" s="10">
         <v>7.9000000000000001E-2</v>
@@ -1596,7 +1465,7 @@
       <c r="H16" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="37" t="s">
         <v>5</v>
       </c>
       <c r="J16" s="10">
@@ -1605,7 +1474,7 @@
       <c r="K16" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L16" s="38" t="s">
+      <c r="L16" s="37" t="s">
         <v>5</v>
       </c>
       <c r="M16" s="10">
@@ -1614,36 +1483,27 @@
       <c r="N16" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="O16" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P16" s="10">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="Q16" s="10">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="R16" s="38" t="s">
+      <c r="O16" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="55" t="s">
-        <v>72</v>
+      <c r="C17" s="54" t="s">
+        <v>67</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="39"/>
+      <c r="F17" s="38"/>
       <c r="G17" s="13">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="H17" s="13">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="38" t="s">
         <v>5</v>
       </c>
       <c r="J17" s="13">
@@ -1652,7 +1512,7 @@
       <c r="K17" s="13">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L17" s="39" t="s">
+      <c r="L17" s="38" t="s">
         <v>5</v>
       </c>
       <c r="M17" s="13">
@@ -1661,36 +1521,27 @@
       <c r="N17" s="13">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="O17" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="P17" s="13">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="Q17" s="13">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="R17" s="39" t="s">
+      <c r="O17" s="38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B18" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="50" t="s">
-        <v>93</v>
+      <c r="C18" s="49" t="s">
+        <v>88</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="40"/>
+      <c r="F18" s="39"/>
       <c r="G18" s="24">
         <v>1.4E-2</v>
       </c>
       <c r="H18" s="24">
         <v>2E-3</v>
       </c>
-      <c r="I18" s="40" t="s">
+      <c r="I18" s="39" t="s">
         <v>5</v>
       </c>
       <c r="J18" s="24">
@@ -1699,7 +1550,7 @@
       <c r="K18" s="24">
         <v>2E-3</v>
       </c>
-      <c r="L18" s="40" t="s">
+      <c r="L18" s="39" t="s">
         <v>5</v>
       </c>
       <c r="M18" s="24">
@@ -1708,36 +1559,27 @@
       <c r="N18" s="24">
         <v>2E-3</v>
       </c>
-      <c r="O18" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="P18" s="24">
-        <v>1.2E-2</v>
-      </c>
-      <c r="Q18" s="24">
-        <v>1E-3</v>
-      </c>
-      <c r="R18" s="40" t="s">
+      <c r="O18" s="39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="50" t="s">
-        <v>80</v>
+        <v>63</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>75</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
-      <c r="F19" s="40"/>
+      <c r="F19" s="39"/>
       <c r="G19" s="24">
         <v>1.4E-2</v>
       </c>
       <c r="H19" s="24">
         <v>2E-3</v>
       </c>
-      <c r="I19" s="40" t="s">
+      <c r="I19" s="39" t="s">
         <v>5</v>
       </c>
       <c r="J19" s="24">
@@ -1746,7 +1588,7 @@
       <c r="K19" s="24">
         <v>2E-3</v>
       </c>
-      <c r="L19" s="40" t="s">
+      <c r="L19" s="39" t="s">
         <v>5</v>
       </c>
       <c r="M19" s="24">
@@ -1755,66 +1597,48 @@
       <c r="N19" s="24">
         <v>2E-3</v>
       </c>
-      <c r="O19" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="P19" s="24">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="Q19" s="24">
-        <v>1E-3</v>
-      </c>
-      <c r="R19" s="40" t="s">
+      <c r="O19" s="39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B20" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>81</v>
+        <v>64</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>76</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
-      <c r="F20" s="40"/>
+      <c r="F20" s="39"/>
       <c r="G20" s="24">
         <v>0</v>
       </c>
       <c r="H20" s="24">
         <v>0</v>
       </c>
-      <c r="I20" s="40"/>
+      <c r="I20" s="39"/>
       <c r="J20" s="24">
         <v>0</v>
       </c>
       <c r="K20" s="24">
         <v>0</v>
       </c>
-      <c r="L20" s="40"/>
+      <c r="L20" s="39"/>
       <c r="M20" s="24">
         <v>0</v>
       </c>
       <c r="N20" s="24">
         <v>0</v>
       </c>
-      <c r="O20" s="40"/>
-      <c r="P20" s="24">
-        <v>1E-3</v>
-      </c>
-      <c r="Q20" s="24">
-        <v>1E-3</v>
-      </c>
-      <c r="R20" s="24" t="s">
-        <v>100</v>
-      </c>
+      <c r="O20" s="39"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B21" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>92</v>
+        <v>59</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>87</v>
       </c>
       <c r="G21" s="10">
         <v>0.497</v>
@@ -1822,7 +1646,7 @@
       <c r="H21" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I21" s="38" t="s">
+      <c r="I21" s="37" t="s">
         <v>5</v>
       </c>
       <c r="J21" s="10">
@@ -1831,7 +1655,7 @@
       <c r="K21" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="L21" s="38" t="s">
+      <c r="L21" s="37" t="s">
         <v>5</v>
       </c>
       <c r="M21" s="10">
@@ -1840,25 +1664,16 @@
       <c r="N21" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="O21" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P21" s="10">
-        <v>0.249</v>
-      </c>
-      <c r="Q21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="R21" s="38" t="s">
+      <c r="O21" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B22" s="36" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="56" t="s">
-        <v>73</v>
+      <c r="C22" s="55" t="s">
+        <v>68</v>
       </c>
       <c r="G22" s="10">
         <v>0.441</v>
@@ -1866,7 +1681,7 @@
       <c r="H22" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I22" s="38" t="s">
+      <c r="I22" s="37" t="s">
         <v>5</v>
       </c>
       <c r="J22" s="10">
@@ -1875,7 +1690,7 @@
       <c r="K22" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="L22" s="38" t="s">
+      <c r="L22" s="37" t="s">
         <v>5</v>
       </c>
       <c r="M22" s="10">
@@ -1884,25 +1699,16 @@
       <c r="N22" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="O22" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P22" s="10">
-        <v>0.20599999999999999</v>
-      </c>
-      <c r="Q22" s="10">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="R22" s="38" t="s">
+      <c r="O22" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B23" s="36" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="51" t="s">
-        <v>91</v>
+      <c r="C23" s="50" t="s">
+        <v>86</v>
       </c>
       <c r="G23" s="10">
         <v>5.7000000000000002E-2</v>
@@ -1910,7 +1716,7 @@
       <c r="H23" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I23" s="38" t="s">
+      <c r="I23" s="37" t="s">
         <v>5</v>
       </c>
       <c r="J23" s="10">
@@ -1919,7 +1725,7 @@
       <c r="K23" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L23" s="38" t="s">
+      <c r="L23" s="37" t="s">
         <v>5</v>
       </c>
       <c r="M23" s="10">
@@ -1928,25 +1734,16 @@
       <c r="N23" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O23" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P23" s="10">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="Q23" s="10">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="R23" s="38" t="s">
+      <c r="O23" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B24" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>82</v>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B24" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>77</v>
       </c>
       <c r="G24" s="10">
         <v>5.6000000000000001E-2</v>
@@ -1954,7 +1751,7 @@
       <c r="H24" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I24" s="38" t="s">
+      <c r="I24" s="37" t="s">
         <v>5</v>
       </c>
       <c r="J24" s="10">
@@ -1963,7 +1760,7 @@
       <c r="K24" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L24" s="38" t="s">
+      <c r="L24" s="37" t="s">
         <v>5</v>
       </c>
       <c r="M24" s="10">
@@ -1972,25 +1769,16 @@
       <c r="N24" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O24" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P24" s="10">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="Q24" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="R24" s="38" t="s">
+      <c r="O24" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B25" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="51" t="s">
-        <v>83</v>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B25" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>78</v>
       </c>
       <c r="G25" s="10">
         <v>1E-3</v>
@@ -2004,7 +1792,7 @@
       <c r="K25" s="10">
         <v>1E-3</v>
       </c>
-      <c r="L25" s="38" t="s">
+      <c r="L25" s="37" t="s">
         <v>9</v>
       </c>
       <c r="M25" s="10">
@@ -2013,25 +1801,16 @@
       <c r="N25" s="10">
         <v>1E-3</v>
       </c>
-      <c r="O25" s="38" t="s">
+      <c r="O25" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="P25" s="10">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="Q25" s="10">
-        <v>2E-3</v>
-      </c>
-      <c r="R25" s="38" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B26" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>84</v>
+        <v>62</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>79</v>
       </c>
       <c r="G26" s="10">
         <v>3.0000000000000001E-3</v>
@@ -2045,7 +1824,7 @@
       <c r="K26" s="14">
         <v>1.2E-2</v>
       </c>
-      <c r="L26" s="38" t="s">
+      <c r="L26" s="37" t="s">
         <v>8</v>
       </c>
       <c r="M26" s="14">
@@ -2054,25 +1833,16 @@
       <c r="N26" s="14">
         <v>1.2E-2</v>
       </c>
-      <c r="O26" s="38" t="s">
+      <c r="O26" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P26" s="10">
-        <v>-3.1E-2</v>
-      </c>
-      <c r="Q26" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="R26" s="38" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B27" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="48" t="s">
-        <v>90</v>
+        <v>60</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>85</v>
       </c>
       <c r="G27" s="10">
         <v>-3.0000000000000001E-3</v>
@@ -2081,7 +1851,7 @@
         <v>2E-3</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J27" s="14">
         <v>-5.0000000000000001E-3</v>
@@ -2089,7 +1859,7 @@
       <c r="K27" s="14">
         <v>2E-3</v>
       </c>
-      <c r="L27" s="38" t="s">
+      <c r="L27" s="37" t="s">
         <v>8</v>
       </c>
       <c r="M27" s="14">
@@ -2098,22 +1868,16 @@
       <c r="N27" s="14">
         <v>2E-3</v>
       </c>
-      <c r="O27" s="38" t="s">
+      <c r="O27" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P27" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="14">
-        <v>2E-3</v>
-      </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B28" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>85</v>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B28" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>80</v>
       </c>
       <c r="G28" s="10">
         <v>-3.0000000000000001E-3</v>
@@ -2122,7 +1886,7 @@
         <v>2E-3</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J28" s="14">
         <v>-5.0000000000000001E-3</v>
@@ -2130,7 +1894,7 @@
       <c r="K28" s="14">
         <v>2E-3</v>
       </c>
-      <c r="L28" s="38" t="s">
+      <c r="L28" s="37" t="s">
         <v>9</v>
       </c>
       <c r="M28" s="14">
@@ -2139,22 +1903,16 @@
       <c r="N28" s="14">
         <v>2E-3</v>
       </c>
-      <c r="O28" s="38" t="s">
+      <c r="O28" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="P28" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="14">
-        <v>2E-3</v>
-      </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B29" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>86</v>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B29" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>81</v>
       </c>
       <c r="G29" s="10">
         <v>0</v>
@@ -2168,7 +1926,7 @@
       <c r="K29" s="14">
         <v>0</v>
       </c>
-      <c r="L29" s="38" t="s">
+      <c r="L29" s="37" t="s">
         <v>9</v>
       </c>
       <c r="M29" s="14">
@@ -2177,22 +1935,16 @@
       <c r="N29" s="14">
         <v>0</v>
       </c>
-      <c r="O29" s="38" t="s">
+      <c r="O29" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="P29" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="14">
-        <v>2E-3</v>
-      </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B30" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="48" t="s">
-        <v>89</v>
+        <v>61</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>84</v>
       </c>
       <c r="G30" s="10">
         <v>5.0000000000000001E-3</v>
@@ -2200,7 +1952,7 @@
       <c r="H30" s="10">
         <v>2E-3</v>
       </c>
-      <c r="I30" s="38" t="s">
+      <c r="I30" s="37" t="s">
         <v>8</v>
       </c>
       <c r="J30" s="10">
@@ -2209,7 +1961,7 @@
       <c r="K30" s="10">
         <v>2E-3</v>
       </c>
-      <c r="L30" s="38" t="s">
+      <c r="L30" s="37" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="10">
@@ -2218,25 +1970,16 @@
       <c r="N30" s="10">
         <v>2E-3</v>
       </c>
-      <c r="O30" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P30" s="14">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="Q30" s="14">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="R30" s="38" t="s">
+      <c r="O30" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B31" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="51" t="s">
-        <v>87</v>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B31" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>82</v>
       </c>
       <c r="G31" s="10">
         <v>4.0000000000000001E-3</v>
@@ -2244,7 +1987,7 @@
       <c r="H31" s="10">
         <v>2E-3</v>
       </c>
-      <c r="I31" s="38" t="s">
+      <c r="I31" s="37" t="s">
         <v>9</v>
       </c>
       <c r="J31" s="10">
@@ -2253,7 +1996,7 @@
       <c r="K31" s="10">
         <v>2E-3</v>
       </c>
-      <c r="L31" s="38" t="s">
+      <c r="L31" s="37" t="s">
         <v>8</v>
       </c>
       <c r="M31" s="10">
@@ -2262,25 +2005,16 @@
       <c r="N31" s="10">
         <v>2E-3</v>
       </c>
-      <c r="O31" s="38" t="s">
+      <c r="O31" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P31" s="10">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="Q31" s="10">
-        <v>2E-3</v>
-      </c>
-      <c r="R31" s="38" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B32" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="51" t="s">
-        <v>88</v>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B32" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="50" t="s">
+        <v>83</v>
       </c>
       <c r="G32" s="10">
         <v>1E-3</v>
@@ -2294,7 +2028,7 @@
       <c r="K32" s="10">
         <v>1E-3</v>
       </c>
-      <c r="L32" s="38" t="s">
+      <c r="L32" s="37" t="s">
         <v>8</v>
       </c>
       <c r="M32" s="10">
@@ -2303,25 +2037,16 @@
       <c r="N32" s="10">
         <v>1E-3</v>
       </c>
-      <c r="O32" s="38" t="s">
+      <c r="O32" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P32" s="10">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="Q32" s="10">
-        <v>2E-3</v>
-      </c>
-      <c r="R32" s="38" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B33" s="11"/>
-      <c r="C33" s="49"/>
+      <c r="C33" s="48"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="16"/>
@@ -2334,16 +2059,13 @@
       <c r="M33" s="11"/>
       <c r="N33" s="11"/>
       <c r="O33" s="16"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="16"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B34" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>101</v>
+      <c r="C34" s="47" t="s">
+        <v>96</v>
       </c>
       <c r="M34" s="10">
         <v>-0.28299999999999997</v>
@@ -2351,25 +2073,16 @@
       <c r="N34" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="O34" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P34" s="10">
-        <v>-0.30299999999999999</v>
-      </c>
-      <c r="Q34" s="10">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="R34" s="38" t="s">
+      <c r="O34" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B35" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="48" t="s">
-        <v>102</v>
+      <c r="C35" s="47" t="s">
+        <v>97</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
@@ -2379,22 +2092,16 @@
       <c r="N35" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="O35" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P35" s="10">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="Q35" s="10">
-        <v>6.3E-2</v>
+      <c r="O35" s="37" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="48" t="s">
-        <v>103</v>
+      <c r="C36" s="47" t="s">
+        <v>98</v>
       </c>
       <c r="M36" s="10">
         <v>0.26600000000000001</v>
@@ -2402,25 +2109,16 @@
       <c r="N36" s="10">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="O36" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P36" s="10">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="Q36" s="10">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="R36" s="38" t="s">
+      <c r="O36" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B37" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="48" t="s">
-        <v>104</v>
+      <c r="C37" s="47" t="s">
+        <v>99</v>
       </c>
       <c r="M37" s="10">
         <v>-0.28699999999999998</v>
@@ -2428,25 +2126,16 @@
       <c r="N37" s="10">
         <v>3.9E-2</v>
       </c>
-      <c r="O37" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P37" s="10">
-        <v>-0.16</v>
-      </c>
-      <c r="Q37" s="10">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="R37" s="38" t="s">
+      <c r="O37" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B38" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="48" t="s">
-        <v>105</v>
+      <c r="C38" s="47" t="s">
+        <v>100</v>
       </c>
       <c r="M38" s="10">
         <v>-0.13</v>
@@ -2454,546 +2143,370 @@
       <c r="N38" s="10">
         <v>1.4E-2</v>
       </c>
-      <c r="O38" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="P38" s="10">
+      <c r="O38" s="37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A39" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A40" s="25"/>
+      <c r="B40" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="51"/>
+      <c r="D40" s="26">
+        <v>6121.9040000000005</v>
+      </c>
+      <c r="E40" s="26">
+        <v>131.19200000000001</v>
+      </c>
+      <c r="F40" s="40"/>
+      <c r="G40" s="26">
+        <v>7856.3670000000002</v>
+      </c>
+      <c r="H40" s="26">
+        <v>114.30500000000001</v>
+      </c>
+      <c r="I40" s="40"/>
+      <c r="J40" s="26">
+        <v>5761.165</v>
+      </c>
+      <c r="K40" s="26">
+        <v>130.59299999999999</v>
+      </c>
+      <c r="L40" s="40"/>
+      <c r="M40" s="26">
+        <v>5761.1769999999997</v>
+      </c>
+      <c r="N40" s="26">
+        <v>130.59399999999999</v>
+      </c>
+      <c r="O40" s="40"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="52"/>
+      <c r="D41" s="18">
+        <v>5240.4769999999999</v>
+      </c>
+      <c r="E41" s="18">
+        <v>202.00399999999999</v>
+      </c>
+      <c r="F41" s="41"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="18">
+        <v>3258.2420000000002</v>
+      </c>
+      <c r="K41" s="18">
+        <v>193.21799999999999</v>
+      </c>
+      <c r="L41" s="41"/>
+      <c r="M41" s="18">
+        <v>1681.29</v>
+      </c>
+      <c r="N41" s="18">
+        <v>138.79499999999999</v>
+      </c>
+      <c r="O41" s="41"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="53"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="42"/>
+      <c r="G42" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="42"/>
+      <c r="J42" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="L42" s="42"/>
+      <c r="M42" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="N42" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="O42" s="42"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A43" s="16"/>
+      <c r="B43" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="22">
+        <v>1253984.4639999999</v>
+      </c>
+      <c r="E43" s="22">
+        <v>1092.7639999999999</v>
+      </c>
+      <c r="F43" s="43"/>
+      <c r="G43" s="22">
+        <v>3420818.0380000002</v>
+      </c>
+      <c r="H43" s="22">
+        <v>1276.701</v>
+      </c>
+      <c r="I43" s="43"/>
+      <c r="J43" s="22">
+        <v>3460679.41</v>
+      </c>
+      <c r="K43" s="22">
+        <v>1253.8389999999999</v>
+      </c>
+      <c r="L43" s="43"/>
+      <c r="M43" s="22">
+        <v>3418712.0010000002</v>
+      </c>
+      <c r="N43" s="22">
+        <v>1240.4179999999999</v>
+      </c>
+      <c r="O43" s="43"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A44" s="16"/>
+      <c r="B44" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="22">
+        <v>1254013.2109999999</v>
+      </c>
+      <c r="E44" s="22">
+        <v>1092.7639999999999</v>
+      </c>
+      <c r="F44" s="43"/>
+      <c r="G44" s="22">
+        <v>3421325.889</v>
+      </c>
+      <c r="H44" s="22">
+        <v>1276.701</v>
+      </c>
+      <c r="I44" s="43"/>
+      <c r="J44" s="22">
+        <v>3461330.9929999998</v>
+      </c>
+      <c r="K44" s="22">
+        <v>1253.8389999999999</v>
+      </c>
+      <c r="L44" s="43"/>
+      <c r="M44" s="22">
+        <v>2419306.091</v>
+      </c>
+      <c r="N44" s="22">
+        <v>1240.4179999999999</v>
+      </c>
+      <c r="O44" s="43"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B45" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="10">
+        <v>2.1930000000000001</v>
+      </c>
+      <c r="E45" s="10">
+        <v>1.468</v>
+      </c>
+      <c r="G45" s="10">
+        <v>358.59899999999999</v>
+      </c>
+      <c r="H45" s="10">
+        <v>13.765000000000001</v>
+      </c>
+      <c r="J45" s="10">
+        <v>231.994</v>
+      </c>
+      <c r="K45" s="10">
+        <v>8.0530000000000008</v>
+      </c>
+      <c r="M45" s="10">
+        <v>261.80900000000003</v>
+      </c>
+      <c r="N45" s="10">
+        <v>8.8979999999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B46" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="10">
+        <v>0</v>
+      </c>
+      <c r="E46" s="10">
+        <v>0</v>
+      </c>
+      <c r="G46" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H46" s="10">
+        <v>0</v>
+      </c>
+      <c r="J46" s="10">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="K46" s="10">
+        <v>0</v>
+      </c>
+      <c r="M46" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="N46" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B47" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0</v>
+      </c>
+      <c r="E47" s="10">
+        <v>0</v>
+      </c>
+      <c r="G47" s="10">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="H47" s="10">
         <v>1E-3</v>
       </c>
-      <c r="Q38" s="10">
-        <v>5.8000000000000003E-2</v>
+      <c r="J47" s="10">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="K47" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="M47" s="10">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="N47" s="10">
+        <v>1E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="16"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="16"/>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B48" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="10">
+        <v>1</v>
+      </c>
+      <c r="E48" s="10">
+        <v>0</v>
+      </c>
+      <c r="G48" s="10">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="H48" s="10">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J48" s="10">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="K48" s="10">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="M48" s="10">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="N48" s="10">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B40" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="P40" s="10">
-        <v>0.70699999999999996</v>
-      </c>
-      <c r="Q40" s="10">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="R40" s="38" t="s">
-        <v>5</v>
-      </c>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A49" s="25"/>
+      <c r="B49" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="51"/>
+      <c r="D49" s="26">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E49" s="26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F49" s="40"/>
+      <c r="G49" s="26">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H49" s="26">
+        <v>0</v>
+      </c>
+      <c r="I49" s="40"/>
+      <c r="J49" s="26">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K49" s="26">
+        <v>0</v>
+      </c>
+      <c r="L49" s="40"/>
+      <c r="M49" s="26">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="N49" s="26">
+        <v>0</v>
+      </c>
+      <c r="O49" s="40"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A41" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="52"/>
-      <c r="D42" s="26">
-        <v>6117.3689999999997</v>
-      </c>
-      <c r="E42" s="26">
-        <v>292.91199999999998</v>
-      </c>
-      <c r="F42" s="41"/>
-      <c r="G42" s="26">
-        <v>7856.3670000000002</v>
-      </c>
-      <c r="H42" s="26">
-        <v>114.30500000000001</v>
-      </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="26">
-        <v>5761.165</v>
-      </c>
-      <c r="K42" s="26">
-        <v>130.59299999999999</v>
-      </c>
-      <c r="L42" s="41"/>
-      <c r="M42" s="26">
-        <v>5761.1769999999997</v>
-      </c>
-      <c r="N42" s="26">
-        <v>130.59399999999999</v>
-      </c>
-      <c r="O42" s="41"/>
-      <c r="P42" s="26">
-        <v>5746.2089999999998</v>
-      </c>
-      <c r="Q42" s="26">
-        <v>249.86099999999999</v>
-      </c>
-      <c r="R42" s="41"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="52"/>
-      <c r="D43" s="26">
-        <v>2657.4430000000002</v>
-      </c>
-      <c r="E43" s="26">
-        <v>329.29399999999998</v>
-      </c>
-      <c r="F43" s="41"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="26">
-        <v>3258.2420000000002</v>
-      </c>
-      <c r="K43" s="26">
-        <v>193.21799999999999</v>
-      </c>
-      <c r="L43" s="41"/>
-      <c r="M43" s="26">
-        <v>1681.29</v>
-      </c>
-      <c r="N43" s="26">
-        <v>138.79499999999999</v>
-      </c>
-      <c r="O43" s="41"/>
-      <c r="P43" s="26">
-        <v>1053.836</v>
-      </c>
-      <c r="Q43" s="26">
-        <v>129.36000000000001</v>
-      </c>
-      <c r="R43" s="41"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="53"/>
-      <c r="D44" s="18">
-        <v>5163.7160000000003</v>
-      </c>
-      <c r="E44" s="18">
-        <v>0.06</v>
-      </c>
-      <c r="F44" s="42"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="42"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="42"/>
-      <c r="P44" s="18">
-        <v>712.71699999999998</v>
-      </c>
-      <c r="Q44" s="18">
-        <v>209.767</v>
-      </c>
-      <c r="R44" s="42"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A45" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="54"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" s="43"/>
-      <c r="G45" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H45" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="K45" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="L45" s="43"/>
-      <c r="M45" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="N45" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="O45" s="43"/>
-      <c r="P45" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q45" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="R45" s="43"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A46" s="16"/>
-      <c r="B46" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="22">
-        <v>1408122.2930000001</v>
-      </c>
-      <c r="E46" s="22">
-        <v>377.19799999999998</v>
-      </c>
-      <c r="F46" s="44"/>
-      <c r="G46" s="22">
-        <v>3420818.0380000002</v>
-      </c>
-      <c r="H46" s="22">
-        <v>1276.701</v>
-      </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="22">
-        <v>3460679.41</v>
-      </c>
-      <c r="K46" s="22">
-        <v>1253.8389999999999</v>
-      </c>
-      <c r="L46" s="44"/>
-      <c r="M46" s="22">
-        <v>3418712.0010000002</v>
-      </c>
-      <c r="N46" s="22">
-        <v>1240.4179999999999</v>
-      </c>
-      <c r="O46" s="44"/>
-      <c r="P46" s="22">
-        <v>3945438.65</v>
-      </c>
-      <c r="Q46" s="22">
-        <v>1028.0650000000001</v>
-      </c>
-      <c r="R46" s="44"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A47" s="16"/>
-      <c r="B47" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" s="22">
-        <v>1408161.0959999999</v>
-      </c>
-      <c r="E47" s="22">
-        <v>377.19799999999998</v>
-      </c>
-      <c r="F47" s="44"/>
-      <c r="G47" s="22">
-        <v>3421325.889</v>
-      </c>
-      <c r="H47" s="22">
-        <v>1276.701</v>
-      </c>
-      <c r="I47" s="44"/>
-      <c r="J47" s="22">
-        <v>3461330.9929999998</v>
-      </c>
-      <c r="K47" s="22">
-        <v>1253.8389999999999</v>
-      </c>
-      <c r="L47" s="44"/>
-      <c r="M47" s="22">
-        <v>2419306.091</v>
-      </c>
-      <c r="N47" s="22">
-        <v>1240.4179999999999</v>
-      </c>
-      <c r="O47" s="44"/>
-      <c r="P47" s="22">
-        <v>3946108.0090000001</v>
-      </c>
-      <c r="Q47" s="22">
-        <v>1028.0650000000001</v>
-      </c>
-      <c r="R47" s="44"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B48" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D48" s="10">
-        <v>30.123999999999999</v>
-      </c>
-      <c r="E48" s="10">
-        <v>3.7570000000000001</v>
-      </c>
-      <c r="G48" s="10">
-        <v>358.59899999999999</v>
-      </c>
-      <c r="H48" s="10">
-        <v>13.765000000000001</v>
-      </c>
-      <c r="J48" s="10">
-        <v>231.994</v>
-      </c>
-      <c r="K48" s="10">
-        <v>8.0530000000000008</v>
-      </c>
-      <c r="M48" s="10">
-        <v>261.80900000000003</v>
-      </c>
-      <c r="N48" s="10">
-        <v>8.8979999999999997</v>
-      </c>
-      <c r="P48" s="10">
-        <v>549.255</v>
-      </c>
-      <c r="Q48" s="10">
-        <v>12.837999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B49" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D49" s="10">
-        <v>0</v>
-      </c>
-      <c r="E49" s="10">
-        <v>0</v>
-      </c>
-      <c r="G49" s="10">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A50" s="17"/>
+      <c r="B50" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="52"/>
+      <c r="D50" s="18">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E50" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F50" s="41"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="18">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H49" s="10">
-        <v>0</v>
-      </c>
-      <c r="J49" s="10">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K49" s="10">
-        <v>0</v>
-      </c>
-      <c r="M49" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="N49" s="10">
-        <v>0</v>
-      </c>
-      <c r="P49" s="10">
-        <v>1.2E-2</v>
-      </c>
-      <c r="Q49" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50" s="10">
-        <v>0</v>
-      </c>
-      <c r="E50" s="10">
-        <v>0</v>
-      </c>
-      <c r="G50" s="10">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="H50" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="J50" s="10">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="K50" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="M50" s="10">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="N50" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="P50" s="10">
-        <v>0.999</v>
-      </c>
-      <c r="Q50" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B51" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="10">
-        <v>1</v>
-      </c>
-      <c r="E51" s="10">
-        <v>0</v>
-      </c>
-      <c r="G51" s="10">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="H51" s="10">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="J51" s="10">
-        <v>0.89200000000000002</v>
-      </c>
-      <c r="K51" s="10">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="M51" s="10">
-        <v>0.90100000000000002</v>
-      </c>
-      <c r="N51" s="10">
+      <c r="K50" s="18">
+        <v>2E-3</v>
+      </c>
+      <c r="L50" s="41"/>
+      <c r="M50" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="N50" s="18">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="P51" s="10">
-        <v>0.998</v>
-      </c>
-      <c r="Q51" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A52" s="25"/>
-      <c r="B52" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52" s="52"/>
-      <c r="D52" s="26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E52" s="26">
-        <v>2E-3</v>
-      </c>
-      <c r="F52" s="41"/>
-      <c r="G52" s="26">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="H52" s="26">
-        <v>0</v>
-      </c>
-      <c r="I52" s="41"/>
-      <c r="J52" s="26">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="K52" s="26">
-        <v>0</v>
-      </c>
-      <c r="L52" s="41"/>
-      <c r="M52" s="26">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="N52" s="26">
-        <v>0</v>
-      </c>
-      <c r="O52" s="41"/>
-      <c r="P52" s="26">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="Q52" s="26">
-        <v>0</v>
-      </c>
-      <c r="R52" s="41"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A53" s="25"/>
-      <c r="B53" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="52"/>
-      <c r="D53" s="26">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="E53" s="26">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="F53" s="41"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="41"/>
-      <c r="J53" s="26">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="K53" s="26">
-        <v>2E-3</v>
-      </c>
-      <c r="L53" s="41"/>
-      <c r="M53" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="N53" s="26">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="O53" s="41"/>
-      <c r="P53" s="26">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="Q53" s="26">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="R53" s="41"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" s="53"/>
-      <c r="D54" s="18">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="E54" s="18">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F54" s="42"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="42"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="42"/>
-      <c r="M54" s="18"/>
-      <c r="N54" s="18"/>
-      <c r="O54" s="42"/>
-      <c r="P54" s="18">
-        <v>0.253</v>
-      </c>
-      <c r="Q54" s="18">
-        <v>1E-3</v>
-      </c>
-      <c r="R54" s="42"/>
+      <c r="O50" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
@@ -3004,10 +2517,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383F5806-D5AD-4D5C-83CF-3D272B6336E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3016,191 +2529,191 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="58" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="58"/>
-    <col min="8" max="8" width="8.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" style="58" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="58"/>
-    <col min="11" max="11" width="8.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" style="58" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="58" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" style="58" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" style="58" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="58" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8" style="58" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" style="58" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" style="58"/>
-    <col min="26" max="26" width="8.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.42578125" style="58" customWidth="1"/>
-    <col min="28" max="28" width="9" style="58" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.85546875" style="58" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.42578125" style="58" customWidth="1"/>
-    <col min="34" max="34" width="8.85546875" style="58" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.85546875" style="58" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4.42578125" style="58" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" style="58"/>
-    <col min="38" max="38" width="5.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4.42578125" style="58" customWidth="1"/>
-    <col min="40" max="40" width="9.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.85546875" style="58" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.42578125" style="58" customWidth="1"/>
-    <col min="43" max="43" width="9.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.42578125" style="58" customWidth="1"/>
-    <col min="46" max="46" width="9.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4.42578125" style="58" customWidth="1"/>
-    <col min="49" max="49" width="9.140625" style="58"/>
-    <col min="50" max="50" width="8.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="4.42578125" style="58" customWidth="1"/>
-    <col min="52" max="52" width="9" style="58" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="6" style="58" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="4.42578125" style="58" customWidth="1"/>
-    <col min="55" max="55" width="9.140625" style="58"/>
-    <col min="56" max="56" width="7.85546875" style="58" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="4.42578125" style="58" customWidth="1"/>
-    <col min="58" max="59" width="9.140625" style="58"/>
-    <col min="60" max="60" width="4.42578125" style="58" customWidth="1"/>
-    <col min="61" max="61" width="8.7109375" style="58" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8" style="58" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="4.42578125" style="58" customWidth="1"/>
-    <col min="64" max="64" width="9" style="58" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.85546875" style="58" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="4.42578125" style="58" customWidth="1"/>
-    <col min="67" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="4.42578125" style="57" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="57"/>
+    <col min="8" max="8" width="8.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" style="57" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="57"/>
+    <col min="11" max="11" width="8.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" style="57" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" style="57" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="57" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="57" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" style="57" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" style="57" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="57"/>
+    <col min="26" max="26" width="8.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.42578125" style="57" customWidth="1"/>
+    <col min="28" max="28" width="9" style="57" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.42578125" style="57" customWidth="1"/>
+    <col min="34" max="34" width="8.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.42578125" style="57" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="57"/>
+    <col min="38" max="38" width="5.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4.42578125" style="57" customWidth="1"/>
+    <col min="40" max="40" width="9.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.42578125" style="57" customWidth="1"/>
+    <col min="43" max="43" width="9.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.42578125" style="57" customWidth="1"/>
+    <col min="46" max="46" width="9.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.42578125" style="57" customWidth="1"/>
+    <col min="49" max="49" width="9.140625" style="57"/>
+    <col min="50" max="50" width="8.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="4.42578125" style="57" customWidth="1"/>
+    <col min="52" max="52" width="9" style="57" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6" style="57" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="4.42578125" style="57" customWidth="1"/>
+    <col min="55" max="55" width="9.140625" style="57"/>
+    <col min="56" max="56" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="4.42578125" style="57" customWidth="1"/>
+    <col min="58" max="59" width="9.140625" style="57"/>
+    <col min="60" max="60" width="4.42578125" style="57" customWidth="1"/>
+    <col min="61" max="61" width="8.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8" style="57" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="4.42578125" style="57" customWidth="1"/>
+    <col min="64" max="64" width="9" style="57" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="4.42578125" style="57" customWidth="1"/>
+    <col min="67" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="35"/>
+      <c r="C1" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="61"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="61"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="61"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="61"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="61"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="35" t="s">
+      <c r="W1" s="61"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="35" t="s">
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="35" t="s">
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="35" t="s">
+      <c r="AF1" s="61"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="35"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="35" t="s">
+      <c r="AI1" s="61"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="35"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="35" t="s">
+      <c r="AL1" s="61"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="35" t="s">
+      <c r="AO1" s="61"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="35" t="s">
+      <c r="AR1" s="61"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="35" t="s">
+      <c r="AU1" s="61"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="35"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="35" t="s">
+      <c r="AX1" s="61"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="35" t="s">
+      <c r="BA1" s="61"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="AO1" s="35"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="35" t="s">
+      <c r="BD1" s="61"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="AR1" s="35"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="35" t="s">
+      <c r="BG1" s="61"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="AU1" s="35"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="35" t="s">
+      <c r="BJ1" s="61"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="AX1" s="35"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="BA1" s="35"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="BD1" s="35"/>
-      <c r="BE1" s="2"/>
-      <c r="BF1" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="BG1" s="35"/>
-      <c r="BH1" s="2"/>
-      <c r="BI1" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="BJ1" s="35"/>
-      <c r="BK1" s="2"/>
-      <c r="BL1" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="BM1" s="35"/>
+      <c r="BM1" s="61"/>
       <c r="BN1" s="2"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="46" t="s">
-        <v>74</v>
+      <c r="C2" s="45" t="s">
+        <v>69</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>1</v>
@@ -3350,12 +2863,12 @@
       </c>
       <c r="BN2" s="5"/>
     </row>
-    <row r="3" spans="1:66" s="59" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:66" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="29"/>
-      <c r="C3" s="47"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
       <c r="F3" s="31"/>
@@ -3602,7 +3115,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="49"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -3672,8 +3185,8 @@
       <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>98</v>
+      <c r="C6" s="47" t="s">
+        <v>93</v>
       </c>
       <c r="D6" s="10">
         <v>-3.2000000000000001E-2</v>
@@ -3846,8 +3359,8 @@
       <c r="B7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
-        <v>70</v>
+      <c r="C7" s="54" t="s">
+        <v>65</v>
       </c>
       <c r="D7" s="13">
         <v>-8.8999999999999996E-2</v>
@@ -4024,8 +3537,8 @@
       <c r="B8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>97</v>
+      <c r="C8" s="49" t="s">
+        <v>92</v>
       </c>
       <c r="D8" s="24">
         <v>5.8000000000000003E-2</v>
@@ -4184,7 +3697,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="BH8" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BI8" s="24">
         <v>8.2000000000000003E-2</v>
@@ -4208,10 +3721,10 @@
     <row r="9" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>76</v>
+        <v>63</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>71</v>
       </c>
       <c r="D9" s="24">
         <v>5.2999999999999999E-2</v>
@@ -4370,7 +3883,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="BH9" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BI9" s="24">
         <v>7.5999999999999998E-2</v>
@@ -4394,10 +3907,10 @@
     <row r="10" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>77</v>
+        <v>64</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>72</v>
       </c>
       <c r="D10" s="24">
         <v>5.0000000000000001E-3</v>
@@ -4521,7 +4034,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AY10" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AZ10" s="24">
         <v>1.6E-2</v>
@@ -4548,7 +4061,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="BH10" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BI10" s="24">
         <v>6.0000000000000001E-3</v>
@@ -4557,7 +4070,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="BK10" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BL10" s="24">
         <v>0</v>
@@ -4572,8 +4085,8 @@
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="48" t="s">
-        <v>96</v>
+      <c r="C11" s="47" t="s">
+        <v>91</v>
       </c>
       <c r="D11" s="10">
         <v>8.9999999999999993E-3</v>
@@ -4742,8 +4255,8 @@
       <c r="B12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="55" t="s">
-        <v>71</v>
+      <c r="C12" s="54" t="s">
+        <v>66</v>
       </c>
       <c r="D12" s="13">
         <v>-1.6E-2</v>
@@ -4752,7 +4265,7 @@
         <v>0.01</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G12" s="13">
         <v>3.6999999999999998E-2</v>
@@ -4777,7 +4290,7 @@
         <v>1.9E-2</v>
       </c>
       <c r="O12" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P12" s="13">
         <v>4.1000000000000002E-2</v>
@@ -4918,8 +4431,8 @@
       <c r="B13" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="50" t="s">
-        <v>95</v>
+      <c r="C13" s="49" t="s">
+        <v>90</v>
       </c>
       <c r="D13" s="24">
         <v>2.5000000000000001E-2</v>
@@ -5102,10 +4615,10 @@
     <row r="14" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>78</v>
+        <v>63</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>73</v>
       </c>
       <c r="D14" s="24">
         <v>0.02</v>
@@ -5262,7 +4775,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="BH14" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BI14" s="24">
         <v>1.4999999999999999E-2</v>
@@ -5286,10 +4799,10 @@
     <row r="15" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>79</v>
+        <v>64</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>74</v>
       </c>
       <c r="D15" s="24">
         <v>5.0000000000000001E-3</v>
@@ -5415,7 +4928,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="AY15" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AZ15" s="24">
         <v>1.4E-2</v>
@@ -5442,7 +4955,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="BH15" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BI15" s="24">
         <v>4.0000000000000001E-3</v>
@@ -5451,7 +4964,7 @@
         <v>2E-3</v>
       </c>
       <c r="BK15" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BL15" s="24">
         <v>1E-3</v>
@@ -5466,8 +4979,8 @@
       <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="56" t="s">
-        <v>94</v>
+      <c r="C16" s="55" t="s">
+        <v>89</v>
       </c>
       <c r="D16" s="10">
         <v>5.5E-2</v>
@@ -5642,8 +5155,8 @@
       <c r="B17" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="55" t="s">
-        <v>72</v>
+      <c r="C17" s="54" t="s">
+        <v>67</v>
       </c>
       <c r="D17" s="13">
         <v>4.5999999999999999E-2</v>
@@ -5818,8 +5331,8 @@
       <c r="B18" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="50" t="s">
-        <v>93</v>
+      <c r="C18" s="49" t="s">
+        <v>88</v>
       </c>
       <c r="D18" s="24">
         <v>0.01</v>
@@ -5837,7 +5350,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J18" s="24">
         <v>5.0000000000000001E-3</v>
@@ -5846,7 +5359,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="L18" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M18" s="24">
         <v>8.9999999999999993E-3</v>
@@ -5992,16 +5505,16 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="BN18" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="50" t="s">
-        <v>80</v>
+        <v>101</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>75</v>
       </c>
       <c r="D19" s="24">
         <v>8.9999999999999993E-3</v>
@@ -6055,7 +5568,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="U19" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="V19" s="24">
         <v>1.2E-2</v>
@@ -6176,16 +5689,16 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="BN19" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>81</v>
+        <v>64</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>76</v>
       </c>
       <c r="D20" s="24">
         <v>0</v>
@@ -6266,7 +5779,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AJ20" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AK20" s="24"/>
       <c r="AL20" s="24"/>
@@ -6342,10 +5855,10 @@
     <row r="21" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>92</v>
+        <v>59</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>87</v>
       </c>
       <c r="D21" s="14">
         <v>0.28999999999999998</v>
@@ -6506,7 +6019,7 @@
         <v>0.122</v>
       </c>
       <c r="BH21" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BI21" s="14">
         <v>0.25</v>
@@ -6532,8 +6045,8 @@
       <c r="B22" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="56" t="s">
-        <v>73</v>
+      <c r="C22" s="55" t="s">
+        <v>68</v>
       </c>
       <c r="D22" s="14">
         <v>0.245</v>
@@ -6694,7 +6207,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="BH22" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BI22" s="14">
         <v>0.22800000000000001</v>
@@ -6720,8 +6233,8 @@
       <c r="B23" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="51" t="s">
-        <v>91</v>
+      <c r="C23" s="50" t="s">
+        <v>86</v>
       </c>
       <c r="D23" s="14">
         <v>4.4999999999999998E-2</v>
@@ -6880,7 +6393,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="BH23" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BI23" s="14">
         <v>2.3E-2</v>
@@ -6904,10 +6417,10 @@
     <row r="24" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>82</v>
+        <v>63</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>77</v>
       </c>
       <c r="D24" s="14">
         <v>0.222</v>
@@ -7066,7 +6579,7 @@
         <v>0.02</v>
       </c>
       <c r="BH24" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BI24" s="14">
         <v>2.1999999999999999E-2</v>
@@ -7090,10 +6603,10 @@
     <row r="25" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="51" t="s">
-        <v>107</v>
+        <v>64</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>102</v>
       </c>
       <c r="D25" s="14">
         <v>6.3E-2</v>
@@ -7257,13 +6770,13 @@
       </c>
       <c r="BN25" s="31"/>
     </row>
-    <row r="26" spans="1:66" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>84</v>
+        <v>62</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>79</v>
       </c>
       <c r="D26" s="14">
         <v>-4.1000000000000002E-2</v>
@@ -7332,7 +6845,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="AD26" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AE26" s="14">
         <v>-8.1000000000000003E-2</v>
@@ -7383,7 +6896,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="AY26" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AZ26" s="14">
         <v>-2.7E-2</v>
@@ -7392,7 +6905,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="BB26" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BC26" s="14">
         <v>-4.0000000000000001E-3</v>
@@ -7428,10 +6941,10 @@
     <row r="27" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="48" t="s">
-        <v>90</v>
+        <v>60</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>85</v>
       </c>
       <c r="D27" s="14">
         <v>-5.0000000000000001E-3</v>
@@ -7590,10 +7103,10 @@
     <row r="28" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>85</v>
+        <v>63</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>80</v>
       </c>
       <c r="D28" s="14">
         <v>-5.0000000000000001E-3</v>
@@ -7639,7 +7152,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="U28" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="V28" s="14">
         <v>-1.0999999999999999E-2</v>
@@ -7737,7 +7250,7 @@
         <v>2E-3</v>
       </c>
       <c r="BK28" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BL28" s="14">
         <v>-8.0000000000000002E-3</v>
@@ -7752,10 +7265,10 @@
     <row r="29" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>86</v>
+        <v>64</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>81</v>
       </c>
       <c r="D29" s="14">
         <v>-1E-3</v>
@@ -7910,10 +7423,10 @@
     <row r="30" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="48" t="s">
-        <v>89</v>
+        <v>61</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>84</v>
       </c>
       <c r="D30" s="14">
         <v>8.0000000000000002E-3</v>
@@ -7963,7 +7476,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="U30" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="V30" s="14">
         <v>2.1000000000000001E-2</v>
@@ -8088,10 +7601,10 @@
     <row r="31" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="51" t="s">
-        <v>87</v>
+        <v>63</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>82</v>
       </c>
       <c r="D31" s="14">
         <v>4.0000000000000001E-3</v>
@@ -8256,10 +7769,10 @@
     <row r="32" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="51" t="s">
-        <v>88</v>
+        <v>64</v>
+      </c>
+      <c r="C32" s="50" t="s">
+        <v>83</v>
       </c>
       <c r="D32" s="14">
         <v>4.0000000000000001E-3</v>
@@ -8385,7 +7898,7 @@
         <v>2E-3</v>
       </c>
       <c r="AY32" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AZ32" s="14">
         <v>1.0999999999999999E-2</v>
@@ -8419,7 +7932,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="BK32" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="BL32" s="14">
         <v>0</v>
@@ -8434,7 +7947,7 @@
         <v>14</v>
       </c>
       <c r="B33" s="11"/>
-      <c r="C33" s="49"/>
+      <c r="C33" s="48"/>
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="33"/>
@@ -8504,8 +8017,8 @@
       <c r="B34" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>101</v>
+      <c r="C34" s="47" t="s">
+        <v>96</v>
       </c>
       <c r="D34" s="30">
         <v>-0.28299999999999997</v>
@@ -8610,7 +8123,7 @@
         <v>0.19400000000000001</v>
       </c>
       <c r="AV34" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AW34" s="30">
         <v>0.23899999999999999</v>
@@ -8660,8 +8173,8 @@
       <c r="B35" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="48" t="s">
-        <v>102</v>
+      <c r="C35" s="47" t="s">
+        <v>97</v>
       </c>
       <c r="D35" s="30">
         <v>-0.214</v>
@@ -8813,8 +8326,8 @@
       <c r="B36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="48" t="s">
-        <v>103</v>
+      <c r="C36" s="47" t="s">
+        <v>98</v>
       </c>
       <c r="D36" s="30">
         <v>0.26600000000000001</v>
@@ -8971,8 +8484,8 @@
       <c r="B37" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="48" t="s">
-        <v>104</v>
+      <c r="C37" s="47" t="s">
+        <v>99</v>
       </c>
       <c r="D37" s="30">
         <v>-0.28699999999999998</v>
@@ -9127,8 +8640,8 @@
       <c r="B38" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="48" t="s">
-        <v>105</v>
+      <c r="C38" s="47" t="s">
+        <v>100</v>
       </c>
       <c r="D38" s="30">
         <v>-0.13</v>
@@ -9181,7 +8694,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="X38" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Y38" s="30">
         <v>3.3000000000000002E-2</v>
@@ -9197,7 +8710,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="AD38" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AE38" s="30">
         <v>9.0999999999999998E-2</v>
@@ -9354,7 +8867,7 @@
       <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="52"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="10">
         <v>5761.1769999999997</v>
       </c>
@@ -9499,12 +9012,12 @@
       </c>
       <c r="BN40" s="10"/>
     </row>
-    <row r="41" spans="1:66" s="61" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:66" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="25"/>
       <c r="B41" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="52"/>
+      <c r="C41" s="51"/>
       <c r="D41" s="26">
         <v>1681.29</v>
       </c>
@@ -9652,7 +9165,7 @@
     <row r="42" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A42" s="17"/>
       <c r="B42" s="17"/>
-      <c r="C42" s="53"/>
+      <c r="C42" s="52"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
@@ -9721,8 +9234,8 @@
       <c r="A43" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="54"/>
-      <c r="C43" s="57"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="56"/>
       <c r="D43" s="19" t="s">
         <v>23</v>
       </c>
@@ -10794,7 +10307,7 @@
       <c r="B50" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="52"/>
+      <c r="C50" s="51"/>
       <c r="D50" s="26">
         <v>1.7000000000000001E-2</v>
       </c>
@@ -10948,7 +10461,7 @@
       <c r="B51" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="53"/>
+      <c r="C51" s="52"/>
       <c r="D51" s="18">
         <v>0.04</v>
       </c>
@@ -11102,6 +10615,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BL1:BM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
@@ -11114,15 +10636,6 @@
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="BF1:BG1"/>
-    <mergeCell ref="BI1:BJ1"/>
-    <mergeCell ref="BL1:BM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BC1:BD1"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Update multilevel multiple imputation data
</commit_message>
<xml_diff>
--- a/Model building/Results 20.xlsx
+++ b/Model building/Results 20.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AC1595-9C67-402E-928D-5FE822B85865}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="640"/>
+    <workbookView xWindow="17895" yWindow="8430" windowWidth="17280" windowHeight="8970" tabRatio="640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Development" sheetId="21" r:id="rId1"/>
     <sheet name="Final" sheetId="22" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -349,7 +350,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -915,11 +916,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
@@ -2517,14 +2518,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:BN51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AK14" sqref="AK14"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -2566,7 +2567,7 @@
     <col min="35" max="35" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="4.42578125" style="57" customWidth="1"/>
     <col min="37" max="37" width="9.140625" style="57"/>
-    <col min="38" max="38" width="5.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6" style="57" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="4.42578125" style="57" customWidth="1"/>
     <col min="40" max="40" width="9.28515625" style="57" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="8.85546875" style="57" bestFit="1" customWidth="1"/>
@@ -10610,20 +10611,8 @@
       </c>
       <c r="BN51" s="18"/>
     </row>
-    <row r="55" spans="1:66" x14ac:dyDescent="0.35">
-      <c r="BN55" s="31"/>
-    </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="BF1:BG1"/>
-    <mergeCell ref="BI1:BJ1"/>
-    <mergeCell ref="BL1:BM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
@@ -10636,6 +10625,15 @@
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BL1:BM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BC1:BD1"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Update Two-saturated: STRATIO with FLSCHOOL EDUSHORT
</commit_message>
<xml_diff>
--- a/Model building/Results 20.xlsx
+++ b/Model building/Results 20.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AC1595-9C67-402E-928D-5FE822B85865}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17895" yWindow="8430" windowWidth="17280" windowHeight="8970" tabRatio="640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17895" yWindow="8430" windowWidth="17280" windowHeight="8970" tabRatio="640"/>
   </bookViews>
   <sheets>
     <sheet name="Model Development" sheetId="21" r:id="rId1"/>
@@ -350,7 +349,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -403,12 +402,18 @@
       <name val="CMU Serif"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -452,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -629,6 +634,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -916,14 +924,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -940,9 +948,9 @@
     <col min="10" max="10" width="9.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.42578125" style="37" customWidth="1"/>
-    <col min="13" max="13" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" style="37" customWidth="1"/>
+    <col min="15" max="15" width="4.140625" style="37" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
@@ -971,11 +979,11 @@
       </c>
       <c r="K1" s="60"/>
       <c r="L1" s="60"/>
-      <c r="M1" s="60" t="s">
+      <c r="M1" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
@@ -1063,10 +1071,10 @@
         <v>5</v>
       </c>
       <c r="M4" s="10">
-        <v>487.29899999999998</v>
+        <v>487.75400000000002</v>
       </c>
       <c r="N4" s="10">
-        <v>4.7949999999999999</v>
+        <v>4.415</v>
       </c>
       <c r="O4" s="37" t="s">
         <v>5</v>
@@ -1117,7 +1125,7 @@
         <v>8</v>
       </c>
       <c r="M6" s="10">
-        <v>-3.2000000000000001E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="N6" s="10">
         <v>1.0999999999999999E-2</v>
@@ -1155,7 +1163,7 @@
         <v>5</v>
       </c>
       <c r="M7" s="13">
-        <v>-8.8999999999999996E-2</v>
+        <v>-9.9000000000000005E-2</v>
       </c>
       <c r="N7" s="13">
         <v>1.0999999999999999E-2</v>
@@ -1193,7 +1201,7 @@
         <v>5</v>
       </c>
       <c r="M8" s="24">
-        <v>5.8000000000000003E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="N8" s="24">
         <v>3.0000000000000001E-3</v>
@@ -1231,7 +1239,7 @@
         <v>5</v>
       </c>
       <c r="M9" s="24">
-        <v>5.2999999999999999E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="N9" s="24">
         <v>3.0000000000000001E-3</v>
@@ -1267,13 +1275,13 @@
         <v>8</v>
       </c>
       <c r="M10" s="24">
-        <v>5.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="N10" s="24">
         <v>2E-3</v>
       </c>
       <c r="O10" s="39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
@@ -1299,7 +1307,7 @@
         <v>0.01</v>
       </c>
       <c r="M11" s="10">
-        <v>8.9999999999999993E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="N11" s="10">
         <v>0.01</v>
@@ -1332,10 +1340,10 @@
         <v>95</v>
       </c>
       <c r="M12" s="13">
-        <v>-1.6E-2</v>
+        <v>-1.7999999999999999E-2</v>
       </c>
       <c r="N12" s="13">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="O12" s="13" t="s">
         <v>95</v>
@@ -1370,7 +1378,7 @@
         <v>5</v>
       </c>
       <c r="M13" s="24">
-        <v>2.5000000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="N13" s="24">
         <v>3.0000000000000001E-3</v>
@@ -1408,7 +1416,7 @@
         <v>5</v>
       </c>
       <c r="M14" s="24">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="N14" s="24">
         <v>2E-3</v>
@@ -1444,13 +1452,13 @@
         <v>8</v>
       </c>
       <c r="M15" s="24">
-        <v>5.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="N15" s="24">
         <v>2E-3</v>
       </c>
       <c r="O15" s="39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
@@ -1479,7 +1487,7 @@
         <v>5</v>
       </c>
       <c r="M16" s="10">
-        <v>5.5E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="N16" s="10">
         <v>8.9999999999999993E-3</v>
@@ -1517,7 +1525,7 @@
         <v>5</v>
       </c>
       <c r="M17" s="13">
-        <v>4.5999999999999999E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="N17" s="13">
         <v>8.9999999999999993E-3</v>
@@ -1593,7 +1601,7 @@
         <v>5</v>
       </c>
       <c r="M19" s="24">
-        <v>8.9999999999999993E-3</v>
+        <v>0.01</v>
       </c>
       <c r="N19" s="24">
         <v>2E-3</v>
@@ -1660,10 +1668,10 @@
         <v>5</v>
       </c>
       <c r="M21" s="10">
-        <v>0.28999999999999998</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="N21" s="10">
-        <v>1.6E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="O21" s="37" t="s">
         <v>5</v>
@@ -1695,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="M22" s="10">
-        <v>0.245</v>
+        <v>0.249</v>
       </c>
       <c r="N22" s="10">
         <v>1.4999999999999999E-2</v>
@@ -1730,7 +1738,7 @@
         <v>5</v>
       </c>
       <c r="M23" s="10">
-        <v>4.4999999999999998E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="N23" s="10">
         <v>3.0000000000000001E-3</v>
@@ -1765,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="M24" s="10">
-        <v>4.2999999999999997E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="N24" s="10">
         <v>3.0000000000000001E-3</v>
@@ -1803,7 +1811,7 @@
         <v>1E-3</v>
       </c>
       <c r="O25" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.35">
@@ -1829,7 +1837,7 @@
         <v>8</v>
       </c>
       <c r="M26" s="14">
-        <v>-4.1000000000000002E-2</v>
+        <v>-3.9E-2</v>
       </c>
       <c r="N26" s="14">
         <v>1.2E-2</v>
@@ -1864,7 +1872,7 @@
         <v>8</v>
       </c>
       <c r="M27" s="14">
-        <v>-5.0000000000000001E-3</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
       <c r="N27" s="14">
         <v>2E-3</v>
@@ -1899,13 +1907,13 @@
         <v>9</v>
       </c>
       <c r="M28" s="14">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="N28" s="14">
         <v>2E-3</v>
       </c>
       <c r="O28" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.35">
@@ -1966,7 +1974,7 @@
         <v>5</v>
       </c>
       <c r="M30" s="10">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="N30" s="10">
         <v>2E-3</v>
@@ -2007,7 +2015,7 @@
         <v>2E-3</v>
       </c>
       <c r="O31" s="37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.35">
@@ -2033,13 +2041,13 @@
         <v>8</v>
       </c>
       <c r="M32" s="10">
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="N32" s="10">
         <v>1E-3</v>
       </c>
       <c r="O32" s="37" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
@@ -2069,7 +2077,7 @@
         <v>96</v>
       </c>
       <c r="M34" s="10">
-        <v>-0.28299999999999997</v>
+        <v>-0.27600000000000002</v>
       </c>
       <c r="N34" s="10">
         <v>6.5000000000000002E-2</v>
@@ -2088,10 +2096,10 @@
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="M35" s="10">
-        <v>-0.214</v>
+        <v>-0.223</v>
       </c>
       <c r="N35" s="10">
-        <v>5.3999999999999999E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="O35" s="37" t="s">
         <v>5</v>
@@ -2105,10 +2113,10 @@
         <v>98</v>
       </c>
       <c r="M36" s="10">
-        <v>0.26600000000000001</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="N36" s="10">
-        <v>7.0999999999999994E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="O36" s="37" t="s">
         <v>5</v>
@@ -2122,10 +2130,10 @@
         <v>99</v>
       </c>
       <c r="M37" s="10">
-        <v>-0.28699999999999998</v>
+        <v>-0.31</v>
       </c>
       <c r="N37" s="10">
-        <v>3.9E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="O37" s="37" t="s">
         <v>5</v>
@@ -2139,10 +2147,10 @@
         <v>100</v>
       </c>
       <c r="M38" s="10">
-        <v>-0.13</v>
+        <v>-0.14199999999999999</v>
       </c>
       <c r="N38" s="10">
-        <v>1.4E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="O38" s="37" t="s">
         <v>5</v>
@@ -2181,10 +2189,10 @@
       </c>
       <c r="L40" s="40"/>
       <c r="M40" s="26">
-        <v>5761.1769999999997</v>
+        <v>5702.2430000000004</v>
       </c>
       <c r="N40" s="26">
-        <v>130.59399999999999</v>
+        <v>127.389</v>
       </c>
       <c r="O40" s="40"/>
     </row>
@@ -2212,10 +2220,10 @@
       </c>
       <c r="L41" s="41"/>
       <c r="M41" s="18">
-        <v>1681.29</v>
+        <v>1584.5119999999999</v>
       </c>
       <c r="N41" s="18">
-        <v>138.79499999999999</v>
+        <v>128.16900000000001</v>
       </c>
       <c r="O41" s="41"/>
     </row>
@@ -2281,10 +2289,10 @@
       </c>
       <c r="L43" s="43"/>
       <c r="M43" s="22">
-        <v>3418712.0010000002</v>
+        <v>3459873.4950000001</v>
       </c>
       <c r="N43" s="22">
-        <v>1240.4179999999999</v>
+        <v>1009.307</v>
       </c>
       <c r="O43" s="43"/>
     </row>
@@ -2315,10 +2323,10 @@
       </c>
       <c r="L44" s="43"/>
       <c r="M44" s="22">
-        <v>2419306.091</v>
+        <v>3460505.9139999999</v>
       </c>
       <c r="N44" s="22">
-        <v>1240.4179999999999</v>
+        <v>1009.307</v>
       </c>
       <c r="O44" s="43"/>
     </row>
@@ -2345,10 +2353,10 @@
         <v>8.0530000000000008</v>
       </c>
       <c r="M45" s="10">
-        <v>261.80900000000003</v>
+        <v>254.97900000000001</v>
       </c>
       <c r="N45" s="10">
-        <v>8.8979999999999997</v>
+        <v>6.4640000000000004</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
@@ -2403,7 +2411,7 @@
         <v>1E-3</v>
       </c>
       <c r="M47" s="10">
-        <v>0.96399999999999997</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="N47" s="10">
         <v>1E-3</v>
@@ -2432,7 +2440,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="M48" s="10">
-        <v>0.90100000000000002</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="N48" s="10">
         <v>3.0000000000000001E-3</v>
@@ -2497,10 +2505,10 @@
       </c>
       <c r="L50" s="41"/>
       <c r="M50" s="18">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="N50" s="18">
-        <v>3.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O50" s="41"/>
     </row>
@@ -2518,10 +2526,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -10613,6 +10621,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BL1:BM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
@@ -10625,15 +10642,6 @@
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="BF1:BG1"/>
-    <mergeCell ref="BI1:BJ1"/>
-    <mergeCell ref="BL1:BM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BC1:BD1"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Add MMI diagnostic data
</commit_message>
<xml_diff>
--- a/Model building/Results 20.xlsx
+++ b/Model building/Results 20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Model building\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E5D871-1E5C-490A-ACDD-3F0D5F4CA2D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AA47D1-AC0F-4600-9F60-B1B1DCA4202B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15915" yWindow="3735" windowWidth="17280" windowHeight="8970" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Development" sheetId="21" r:id="rId1"/>
@@ -266,9 +266,6 @@
     <t>γ₄₁β₁</t>
   </si>
   <si>
-    <t>γ₄₁β₂</t>
-  </si>
-  <si>
     <t>γ₅</t>
   </si>
   <si>
@@ -340,6 +337,28 @@
   <si>
     <t>γ₄₂β₂</t>
   </si>
+  <si>
+    <r>
+      <t>γ₄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>₂</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMU Serif"/>
+      </rPr>
+      <t>β₂</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -348,7 +367,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,6 +414,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="CMU Serif"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -914,33 +939,33 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:O50"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="10"/>
-    <col min="5" max="5" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" style="37" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="10"/>
+    <col min="5" max="5" width="8.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.44140625" style="37" customWidth="1"/>
     <col min="7" max="7" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" style="37" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" style="37" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.140625" style="37" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="53"/>
+    <col min="8" max="8" width="8.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.44140625" style="37" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.44140625" style="37" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.109375" style="37" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="34"/>
       <c r="B1" s="1"/>
       <c r="C1" s="44" t="s">
@@ -967,7 +992,7 @@
       <c r="N1" s="60"/>
       <c r="O1" s="60"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="45" t="s">
@@ -1002,7 +1027,7 @@
       </c>
       <c r="O2" s="36"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1046,7 @@
       <c r="N3" s="8"/>
       <c r="O3" s="31"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1062,7 +1087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -1081,12 +1106,12 @@
       <c r="N5" s="11"/>
       <c r="O5" s="16"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6" s="10">
         <v>-7.2999999999999995E-2</v>
@@ -1116,7 +1141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B7" s="12" t="s">
         <v>10</v>
       </c>
@@ -1154,12 +1179,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B8" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
@@ -1192,7 +1217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B9" s="23" t="s">
         <v>61</v>
       </c>
@@ -1230,7 +1255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B10" s="23" t="s">
         <v>62</v>
       </c>
@@ -1266,12 +1291,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G11" s="10">
         <v>8.0000000000000002E-3</v>
@@ -1293,7 +1318,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B12" s="12" t="s">
         <v>10</v>
       </c>
@@ -1331,12 +1356,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B13" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
@@ -1369,7 +1394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B14" s="23" t="s">
         <v>61</v>
       </c>
@@ -1407,7 +1432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B15" s="23" t="s">
         <v>62</v>
       </c>
@@ -1443,12 +1468,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="10">
         <v>7.4999999999999997E-2</v>
@@ -1478,7 +1503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B17" s="12" t="s">
         <v>10</v>
       </c>
@@ -1516,12 +1541,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B18" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
@@ -1554,7 +1579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B19" s="23" t="s">
         <v>61</v>
       </c>
@@ -1592,7 +1617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B20" s="23" t="s">
         <v>62</v>
       </c>
@@ -1624,12 +1649,12 @@
       </c>
       <c r="O20" s="39"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B21" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21" s="10">
         <v>0.497</v>
@@ -1659,7 +1684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B22" s="35" t="s">
         <v>10</v>
       </c>
@@ -1694,12 +1719,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B23" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G23" s="10">
         <v>5.1999999999999998E-2</v>
@@ -1729,7 +1754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B24" s="35" t="s">
         <v>61</v>
       </c>
@@ -1764,12 +1789,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B25" s="35" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="G25" s="10">
         <v>1E-3</v>
@@ -1796,12 +1821,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B26" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G26" s="10">
         <v>4.0000000000000001E-3</v>
@@ -1828,12 +1853,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B27" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G27" s="10">
         <v>-3.0000000000000001E-3</v>
@@ -1842,7 +1867,7 @@
         <v>2E-3</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J27" s="14">
         <v>-6.0000000000000001E-3</v>
@@ -1863,12 +1888,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B28" s="35" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G28" s="10">
         <v>-3.0000000000000001E-3</v>
@@ -1877,7 +1902,7 @@
         <v>2E-3</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J28" s="14">
         <v>-5.0000000000000001E-3</v>
@@ -1898,12 +1923,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B29" s="35" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G29" s="10">
         <v>0</v>
@@ -1930,12 +1955,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B30" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G30" s="10">
         <v>4.0000000000000001E-3</v>
@@ -1965,12 +1990,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B31" s="35" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G31" s="10">
         <v>3.0000000000000001E-3</v>
@@ -2000,12 +2025,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B32" s="35" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G32" s="10">
         <v>1E-3</v>
@@ -2032,7 +2057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A33" s="11" t="s">
         <v>14</v>
       </c>
@@ -2051,12 +2076,12 @@
       <c r="N33" s="11"/>
       <c r="O33" s="16"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B34" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M34" s="10">
         <v>-0.29499999999999998</v>
@@ -2068,12 +2093,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B35" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
@@ -2087,12 +2112,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B36" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M36" s="10">
         <v>0.23300000000000001</v>
@@ -2104,12 +2129,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B37" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C37" s="47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M37" s="10">
         <v>-0.29199999999999998</v>
@@ -2121,12 +2146,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B38" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M38" s="10">
         <v>-0.13200000000000001</v>
@@ -2138,12 +2163,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A39" s="16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A40" s="25"/>
       <c r="B40" s="25" t="s">
         <v>20</v>
@@ -2178,7 +2203,7 @@
       </c>
       <c r="O40" s="40"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A41" s="17"/>
       <c r="B41" s="17" t="s">
         <v>21</v>
@@ -2209,7 +2234,7 @@
       </c>
       <c r="O41" s="41"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>
@@ -2244,7 +2269,7 @@
       </c>
       <c r="O42" s="42"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A43" s="16"/>
       <c r="B43" s="9" t="s">
         <v>25</v>
@@ -2278,7 +2303,7 @@
       </c>
       <c r="O43" s="43"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A44" s="16"/>
       <c r="B44" s="9" t="s">
         <v>26</v>
@@ -2312,7 +2337,7 @@
       </c>
       <c r="O44" s="43"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B45" s="9" t="s">
         <v>27</v>
       </c>
@@ -2341,7 +2366,7 @@
         <v>11.746</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B46" s="9" t="s">
         <v>28</v>
       </c>
@@ -2370,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B47" s="9" t="s">
         <v>29</v>
       </c>
@@ -2399,7 +2424,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B48" s="9" t="s">
         <v>30</v>
       </c>
@@ -2428,7 +2453,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A49" s="25"/>
       <c r="B49" s="25" t="s">
         <v>31</v>
@@ -2463,7 +2488,7 @@
       </c>
       <c r="O49" s="40"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A50" s="17"/>
       <c r="B50" s="17" t="s">
         <v>32</v>
@@ -2518,84 +2543,84 @@
       <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="57" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="57" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="47" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="57" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="57"/>
+    <col min="5" max="5" width="8.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="57"/>
     <col min="8" max="8" width="9" style="57" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" style="57" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="57"/>
-    <col min="11" max="11" width="8.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" style="57" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" style="57" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.44140625" style="57" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="57"/>
+    <col min="11" max="11" width="8.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.44140625" style="57" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.44140625" style="57" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="57" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="57" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.109375" style="57" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="57" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="57" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.44140625" style="57" customWidth="1"/>
+    <col min="22" max="22" width="9.44140625" style="57" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8" style="57" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.42578125" style="57" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" style="57"/>
-    <col min="26" max="26" width="8.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.42578125" style="57" customWidth="1"/>
+    <col min="24" max="24" width="4.44140625" style="57" customWidth="1"/>
+    <col min="25" max="25" width="9.109375" style="57"/>
+    <col min="26" max="26" width="8.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.44140625" style="57" customWidth="1"/>
     <col min="28" max="28" width="9" style="57" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.109375" style="57" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" style="57" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.42578125" style="57" customWidth="1"/>
-    <col min="34" max="34" width="8.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4.42578125" style="57" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" style="57"/>
-    <col min="38" max="38" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4.42578125" style="57" customWidth="1"/>
-    <col min="40" max="40" width="9.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.42578125" style="57" customWidth="1"/>
-    <col min="43" max="43" width="9.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.42578125" style="57" customWidth="1"/>
-    <col min="46" max="46" width="9.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4.42578125" style="57" customWidth="1"/>
-    <col min="49" max="49" width="9.140625" style="57"/>
-    <col min="50" max="50" width="8.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="4.42578125" style="57" customWidth="1"/>
+    <col min="32" max="32" width="9.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.44140625" style="57" customWidth="1"/>
+    <col min="34" max="34" width="8.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.44140625" style="57" customWidth="1"/>
+    <col min="37" max="37" width="9.109375" style="57"/>
+    <col min="38" max="38" width="7.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4.44140625" style="57" customWidth="1"/>
+    <col min="40" max="40" width="9.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.44140625" style="57" customWidth="1"/>
+    <col min="43" max="43" width="9.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.44140625" style="57" customWidth="1"/>
+    <col min="46" max="46" width="9.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.44140625" style="57" customWidth="1"/>
+    <col min="49" max="49" width="9.109375" style="57"/>
+    <col min="50" max="50" width="8.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="4.44140625" style="57" customWidth="1"/>
     <col min="52" max="52" width="9" style="57" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="4.42578125" style="57" customWidth="1"/>
-    <col min="55" max="55" width="9.140625" style="57"/>
-    <col min="56" max="56" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="4.42578125" style="57" customWidth="1"/>
-    <col min="58" max="59" width="9.140625" style="57"/>
-    <col min="60" max="60" width="4.42578125" style="57" customWidth="1"/>
-    <col min="61" max="61" width="8.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="4.44140625" style="57" customWidth="1"/>
+    <col min="55" max="55" width="9.109375" style="57"/>
+    <col min="56" max="56" width="7.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="4.44140625" style="57" customWidth="1"/>
+    <col min="58" max="59" width="9.109375" style="57"/>
+    <col min="60" max="60" width="4.44140625" style="57" customWidth="1"/>
+    <col min="61" max="61" width="8.6640625" style="57" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="8" style="57" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="4.42578125" style="57" customWidth="1"/>
+    <col min="63" max="63" width="4.44140625" style="57" customWidth="1"/>
     <col min="64" max="64" width="9" style="57" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="7.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="4.42578125" style="57" customWidth="1"/>
-    <col min="67" max="16384" width="9.140625" style="57"/>
+    <col min="65" max="65" width="7.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="4.44140625" style="57" customWidth="1"/>
+    <col min="67" max="16384" width="9.109375" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="44" t="s">
         <v>68</v>
       </c>
       <c r="D1" s="61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="61"/>
       <c r="F1" s="2"/>
@@ -2700,7 +2725,7 @@
       <c r="BM1" s="61"/>
       <c r="BN1" s="2"/>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="45" t="s">
@@ -2854,7 +2879,7 @@
       </c>
       <c r="BN2" s="5"/>
     </row>
-    <row r="3" spans="1:66" s="58" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:66" s="58" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -2930,7 +2955,7 @@
       <c r="BM3" s="30"/>
       <c r="BN3" s="31"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A4" s="9"/>
       <c r="B4" s="9" t="s">
         <v>4</v>
@@ -2951,7 +2976,7 @@
         <v>279.74</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J4" s="10">
         <v>344.03899999999999</v>
@@ -3105,7 +3130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -3175,13 +3200,13 @@
       <c r="BM5" s="11"/>
       <c r="BN5" s="11"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" s="10">
         <v>-3.5999999999999997E-2</v>
@@ -3347,7 +3372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A7" s="9"/>
       <c r="B7" s="12" t="s">
         <v>10</v>
@@ -3405,7 +3430,7 @@
         <v>0.02</v>
       </c>
       <c r="U7" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V7" s="13">
         <v>0.08</v>
@@ -3457,7 +3482,7 @@
         <v>1.9E-2</v>
       </c>
       <c r="AM7" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AN7" s="13">
         <v>-3.0000000000000001E-3</v>
@@ -3529,13 +3554,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A8" s="9"/>
       <c r="B8" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="24">
         <v>5.1999999999999998E-2</v>
@@ -3717,7 +3742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A9" s="9"/>
       <c r="B9" s="23" t="s">
         <v>61</v>
@@ -3905,7 +3930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A10" s="9"/>
       <c r="B10" s="23" t="s">
         <v>62</v>
@@ -3970,7 +3995,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="X10" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Y10" s="24">
         <v>4.0000000000000001E-3</v>
@@ -4085,13 +4110,13 @@
       </c>
       <c r="BN10" s="24"/>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="10">
         <v>5.0000000000000001E-3</v>
@@ -4253,7 +4278,7 @@
       </c>
       <c r="BN11" s="10"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A12" s="9"/>
       <c r="B12" s="12" t="s">
         <v>10</v>
@@ -4291,7 +4316,7 @@
         <v>2.3E-2</v>
       </c>
       <c r="O12" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P12" s="13">
         <v>4.1000000000000002E-2</v>
@@ -4427,13 +4452,13 @@
       </c>
       <c r="BN12" s="13"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A13" s="9"/>
       <c r="B13" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="24">
         <v>2.4E-2</v>
@@ -4613,7 +4638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A14" s="9"/>
       <c r="B14" s="23" t="s">
         <v>61</v>
@@ -4799,7 +4824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A15" s="9"/>
       <c r="B15" s="23" t="s">
         <v>62</v>
@@ -4977,13 +5002,13 @@
       </c>
       <c r="BN15" s="24"/>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A16" s="9"/>
       <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="10">
         <v>5.2999999999999999E-2</v>
@@ -5118,7 +5143,7 @@
         <v>0.02</v>
       </c>
       <c r="BB16" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BC16" s="10">
         <v>5.0999999999999997E-2</v>
@@ -5157,7 +5182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A17" s="9"/>
       <c r="B17" s="12" t="s">
         <v>10</v>
@@ -5206,7 +5231,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S17" s="13">
         <v>2.5999999999999999E-2</v>
@@ -5305,7 +5330,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="BE17" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BF17" s="13">
         <v>8.1000000000000003E-2</v>
@@ -5335,13 +5360,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A18" s="9"/>
       <c r="B18" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" s="24">
         <v>7.0000000000000001E-3</v>
@@ -5412,7 +5437,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AD18" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AE18" s="24">
         <v>7.0000000000000001E-3</v>
@@ -5513,10 +5538,10 @@
       </c>
       <c r="BN18" s="24"/>
     </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A19" s="9"/>
       <c r="B19" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="49" t="s">
         <v>73</v>
@@ -5588,7 +5613,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AD19" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AE19" s="24">
         <v>7.0000000000000001E-3</v>
@@ -5687,7 +5712,7 @@
       </c>
       <c r="BN19" s="24"/>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A20" s="9"/>
       <c r="B20" s="23" t="s">
         <v>62</v>
@@ -5774,7 +5799,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AJ20" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AK20" s="24">
         <v>3.0000000000000001E-3</v>
@@ -5783,7 +5808,7 @@
         <v>2E-3</v>
       </c>
       <c r="AM20" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AN20" s="24">
         <v>2E-3</v>
@@ -5849,13 +5874,13 @@
       </c>
       <c r="BN20" s="24"/>
     </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A21" s="9"/>
       <c r="B21" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="14">
         <v>0.28899999999999998</v>
@@ -6037,7 +6062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A22" s="9"/>
       <c r="B22" s="28" t="s">
         <v>10</v>
@@ -6122,7 +6147,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="AD22" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AE22" s="14">
         <v>6.9000000000000006E-2</v>
@@ -6225,13 +6250,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A23" s="9"/>
       <c r="B23" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D23" s="14">
         <v>4.1000000000000002E-2</v>
@@ -6413,7 +6438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A24" s="9"/>
       <c r="B24" s="28" t="s">
         <v>61</v>
@@ -6601,13 +6626,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A25" s="9"/>
       <c r="B25" s="28" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" s="14">
         <v>1E-3</v>
@@ -6754,7 +6779,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="BH25" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BI25" s="14">
         <v>1E-3</v>
@@ -6771,13 +6796,13 @@
       </c>
       <c r="BN25" s="31"/>
     </row>
-    <row r="26" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="9"/>
       <c r="B26" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="14">
         <v>-0.04</v>
@@ -6933,13 +6958,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A27" s="9"/>
       <c r="B27" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" s="14">
         <v>-6.0000000000000001E-3</v>
@@ -7095,13 +7120,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A28" s="9"/>
       <c r="B28" s="28" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="14">
         <v>-5.0000000000000001E-3</v>
@@ -7147,7 +7172,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="U28" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V28" s="14">
         <v>-1.2E-2</v>
@@ -7245,7 +7270,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="BK28" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BL28" s="14">
         <v>-8.0000000000000002E-3</v>
@@ -7257,13 +7282,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A29" s="9"/>
       <c r="B29" s="28" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" s="14">
         <v>-1E-3</v>
@@ -7339,7 +7364,7 @@
         <v>1E-3</v>
       </c>
       <c r="AG29" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AH29" s="14">
         <v>-1E-3</v>
@@ -7415,13 +7440,13 @@
       </c>
       <c r="BN29" s="32"/>
     </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A30" s="9"/>
       <c r="B30" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D30" s="14">
         <v>7.0000000000000001E-3</v>
@@ -7471,7 +7496,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="U30" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V30" s="14">
         <v>2.1999999999999999E-2</v>
@@ -7567,7 +7592,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="BE30" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BF30" s="14">
         <v>8.9999999999999993E-3</v>
@@ -7576,7 +7601,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="BH30" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BI30" s="14">
         <v>3.0000000000000001E-3</v>
@@ -7595,13 +7620,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A31" s="9"/>
       <c r="B31" s="28" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="14">
         <v>4.0000000000000001E-3</v>
@@ -7626,7 +7651,7 @@
         <v>2E-3</v>
       </c>
       <c r="L31" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M31" s="14">
         <v>2.3E-2</v>
@@ -7644,7 +7669,7 @@
         <v>2E-3</v>
       </c>
       <c r="R31" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S31" s="14">
         <v>-2E-3</v>
@@ -7767,13 +7792,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A32" s="9"/>
       <c r="B32" s="28" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" s="14">
         <v>3.0000000000000001E-3</v>
@@ -7832,7 +7857,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="X32" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Y32" s="14">
         <v>2E-3</v>
@@ -7945,7 +7970,7 @@
       </c>
       <c r="BN32" s="14"/>
     </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A33" s="11" t="s">
         <v>14</v>
       </c>
@@ -8015,13 +8040,13 @@
       <c r="BM33" s="33"/>
       <c r="BN33" s="33"/>
     </row>
-    <row r="34" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="9"/>
       <c r="B34" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D34" s="30">
         <v>-0.29499999999999998</v>
@@ -8132,7 +8157,7 @@
         <v>0.2</v>
       </c>
       <c r="AV34" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AW34" s="30"/>
       <c r="AX34" s="30"/>
@@ -8175,13 +8200,13 @@
       </c>
       <c r="BN34" s="31"/>
     </row>
-    <row r="35" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D35" s="30">
         <v>-0.22500000000000001</v>
@@ -8331,13 +8356,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D36" s="30">
         <v>0.23300000000000001</v>
@@ -8489,13 +8514,13 @@
       </c>
       <c r="BN36" s="31"/>
     </row>
-    <row r="37" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="9"/>
       <c r="B37" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C37" s="47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D37" s="30">
         <v>-0.29199999999999998</v>
@@ -8645,13 +8670,13 @@
       </c>
       <c r="BN37" s="31"/>
     </row>
-    <row r="38" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:66" s="53" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="9"/>
       <c r="B38" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D38" s="30">
         <v>-0.13200000000000001</v>
@@ -8799,7 +8824,7 @@
       </c>
       <c r="BN38" s="31"/>
     </row>
-    <row r="39" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A39" s="16" t="s">
         <v>36</v>
       </c>
@@ -8868,7 +8893,7 @@
       <c r="BM39" s="14"/>
       <c r="BN39" s="14"/>
     </row>
-    <row r="40" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A40" s="25"/>
       <c r="B40" s="25" t="s">
         <v>20</v>
@@ -9018,7 +9043,7 @@
       </c>
       <c r="BN40" s="26"/>
     </row>
-    <row r="41" spans="1:66" s="59" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:66" s="59" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="17"/>
       <c r="B41" s="17" t="s">
         <v>21</v>
@@ -9168,7 +9193,7 @@
       </c>
       <c r="BN41" s="18"/>
     </row>
-    <row r="42" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>
@@ -9322,7 +9347,7 @@
       </c>
       <c r="BN42" s="21"/>
     </row>
-    <row r="43" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A43" s="16"/>
       <c r="B43" s="9" t="s">
         <v>25</v>
@@ -9475,7 +9500,7 @@
       </c>
       <c r="BN43" s="22"/>
     </row>
-    <row r="44" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A44" s="16"/>
       <c r="B44" s="9" t="s">
         <v>26</v>
@@ -9628,7 +9653,7 @@
       </c>
       <c r="BN44" s="22"/>
     </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A45" s="9"/>
       <c r="B45" s="9" t="s">
         <v>27</v>
@@ -9781,7 +9806,7 @@
       </c>
       <c r="BN45" s="10"/>
     </row>
-    <row r="46" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A46" s="9"/>
       <c r="B46" s="9" t="s">
         <v>28</v>
@@ -9934,7 +9959,7 @@
       </c>
       <c r="BN46" s="10"/>
     </row>
-    <row r="47" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A47" s="9"/>
       <c r="B47" s="9" t="s">
         <v>29</v>
@@ -10087,7 +10112,7 @@
       </c>
       <c r="BN47" s="10"/>
     </row>
-    <row r="48" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A48" s="9"/>
       <c r="B48" s="9" t="s">
         <v>30</v>
@@ -10240,7 +10265,7 @@
       </c>
       <c r="BN48" s="10"/>
     </row>
-    <row r="49" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A49" s="25"/>
       <c r="B49" s="25" t="s">
         <v>31</v>
@@ -10394,7 +10419,7 @@
       </c>
       <c r="BN49" s="26"/>
     </row>
-    <row r="50" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:66" x14ac:dyDescent="0.4">
       <c r="A50" s="17"/>
       <c r="B50" s="17" t="s">
         <v>32</v>
@@ -10550,15 +10575,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="BF1:BG1"/>
-    <mergeCell ref="BI1:BJ1"/>
-    <mergeCell ref="BL1:BM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
@@ -10571,6 +10587,15 @@
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BL1:BM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BC1:BD1"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>